<commit_message>
Complete Overhead Signs 2020 links
Streetview links for Overhead Signs FY 2020 maintenance is complete.
</commit_message>
<xml_diff>
--- a/OverheadSigns/OverheadSigns_FY2020.xlsx
+++ b/OverheadSigns/OverheadSigns_FY2020.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="969">
   <si>
     <t>COA_INTERSECTION_ID</t>
   </si>
@@ -4740,6 +4740,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/CS19pRmU3gJvKiSv9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/7Y12NQ8tbZDtrHiz8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/xVxF4b3tUmHAKMCE9</t>
+    </r>
+  </si>
+  <si>
     <t>659</t>
   </si>
   <si>
@@ -4780,6 +4813,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/W7UxkkJhqgTgNyT17</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5mYp1amfqHR7CKJ17</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/F8bpjpz4z4XAN4kT9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/KHrbz8LRWemLN83QA</t>
+    </r>
+  </si>
+  <si>
     <t>838</t>
   </si>
   <si>
@@ -4800,6 +4877,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/hfT1DmqpAnDbTo9Z7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ZMWFV1TCHDSywfrq5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ESC88einSeu47hNv8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/Dsc8t3zEiNfS5sHg8</t>
+    </r>
+  </si>
+  <si>
     <t>860</t>
   </si>
   <si>
@@ -4820,6 +4941,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/EedipFgGpoZ7R4UX9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/FgihyCUixopkwFBK8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/Uw5AsZ1zKvdY9i5t5</t>
+    </r>
+  </si>
+  <si>
     <t>197</t>
   </si>
   <si>
@@ -4840,6 +4994,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/aghpT5hHmPWqHyhB7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/pGMuWGUR55dmvQ1s5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/sUe4WPttT8djc8y88</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/AaZBhvMWLyrDaxsL8</t>
+    </r>
+  </si>
+  <si>
     <t>753</t>
   </si>
   <si>
@@ -4860,6 +5058,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ZMXdf3m5B9sNkGWFA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/PZV1WZuVL9BzTK4Z8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/4JoSKjZxQsFXn49v6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/uh22JNTVD1wpJ6qi8</t>
+    </r>
+  </si>
+  <si>
     <t>109</t>
   </si>
   <si>
@@ -4880,6 +5122,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/jHXmuhJLxkDfMjxi7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/gXqKjgArVTWE18X67</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/J2DKCiHvVs1PtBDS8</t>
+    </r>
+  </si>
+  <si>
     <t>164</t>
   </si>
   <si>
@@ -4900,6 +5175,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/YnMYTqrysmZeNCmw8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/T4bEb9dxN8tj4fUG7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/PJ2zUC7dxZHgRroS7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/DzgXDnjtxeZihT2s5</t>
+    </r>
+  </si>
+  <si>
     <t>513</t>
   </si>
   <si>
@@ -4920,6 +5239,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/xJEZScTM3jd31vjv7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/7igom4JU6M4SNSuBA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ESTyDw9Lut2NS5Hs9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/KAPdszwxyKekKeaz7</t>
+    </r>
+  </si>
+  <si>
     <t>665</t>
   </si>
   <si>
@@ -4940,6 +5303,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/Y5VnGD6uDHWBNnX18</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/WUcmGJsgfRU2mSDLA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/v3aTBeaPY8xay8H78</t>
+    </r>
+  </si>
+  <si>
     <t>110</t>
   </si>
   <si>
@@ -4960,6 +5356,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/bD5sgWGFfpPR3g6G8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/q4C3jXjr6U9KavAu6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/q51dSkwJwMzQBsod6</t>
+    </r>
+  </si>
+  <si>
     <t>172</t>
   </si>
   <si>
@@ -4980,6 +5409,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/auCxBooZmFBN6moA9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/AdVE4j5KNAqK3PZy5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/tmTrmsuNtbW9fj3i7</t>
+    </r>
+  </si>
+  <si>
     <t>208</t>
   </si>
   <si>
@@ -5000,6 +5462,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/S47N95nvEgJiveT1A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/xDbHjRoqKYdCa55g9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/aoKoSpsUKKyAh4ez6</t>
+    </r>
+  </si>
+  <si>
     <t>214</t>
   </si>
   <si>
@@ -5020,6 +5515,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/z4dwugxPNoPRyLzV7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/QbB6B5XNEzRPLcRW6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/fcBcNbaxxYwhz5NA7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/DFU3CVug9eL7srUr7</t>
+    </r>
+  </si>
+  <si>
     <t>421</t>
   </si>
   <si>
@@ -5040,6 +5579,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/19AXTpeHCQAS9d6m9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/uWpGrAuSPSMG71mJA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/kRFE8fvmB7HwQe2E8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/RjxBLNgiN55phzrU7</t>
+    </r>
+  </si>
+  <si>
     <t>423</t>
   </si>
   <si>
@@ -5060,6 +5643,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/vzwq8aW5mKKc5DgJ8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/vNNzLE8MaTEkmsBV6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/KZxRXdQTzbqtBJMz7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/vU2yu3nvERJDkhdc9</t>
+    </r>
+  </si>
+  <si>
     <t>658</t>
   </si>
   <si>
@@ -5080,6 +5707,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/WBgpBev5rPLWwjP38</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/6CsB2w6jrVswkrrd8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/fTH5RoqhmhGeFw6b7</t>
+    </r>
+  </si>
+  <si>
     <t>706</t>
   </si>
   <si>
@@ -5100,6 +5760,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/eSGV5XZLEGWhQexZ6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/XeGwregfm1xHc9Hm8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/MaJWfHaZDKjN252U8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/T9vHpRYJg6moH5hH7</t>
+    </r>
+  </si>
+  <si>
     <t>711</t>
   </si>
   <si>
@@ -5120,15 +5824,125 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/DMPSctVAjFQCY9Rh8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/aoxZQED2KcPQ6zfS9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/QqLPFb67qcmfvsbD9</t>
+    </r>
+  </si>
+  <si>
     <t>789</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/DoKyNBiWYqZCiLKW6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/C1Yfhnw6pFdKKT6s5</t>
+    </r>
+  </si>
+  <si>
     <t>790</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/J2PArsKwDnzNsfnq7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/8x5AigDmeCx2Qxsm7</t>
+    </r>
+  </si>
+  <si>
     <t>794</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/P8CR1UKYEbrXCka4A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/AMfTdUj5P5ipvTyg9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/QRqgFYhSBYVNHBS87</t>
+    </r>
+  </si>
+  <si>
     <t>851</t>
   </si>
   <si>
@@ -5149,6 +5963,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/56dbeokQKXSUpF7BA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/znKJA51SgWj84QrF8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/iMcm945afhbM9EiB9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/iz29tDGmqTENPUNv6</t>
+    </r>
+  </si>
+  <si>
     <t>949</t>
   </si>
   <si>
@@ -5169,9 +6027,86 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/RT7m4Y3Fu1yGRGP58</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/shuwK4WWkyqenC9R6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/nDLurtQfMcrpZxh56</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/xSUAH6aRJpu97wEL9</t>
+    </r>
+  </si>
+  <si>
     <t>955</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5iD4jhvXe1LEejHf9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/KJjsfEVd2n7TSmrE7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5Jc4UZHzqZzbfDMo6</t>
+    </r>
+  </si>
+  <si>
     <t>1004</t>
   </si>
   <si>
@@ -5192,6 +6127,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/sBonvkz7BpL5qfv28</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/wzz6E4jL3DuBuYaUA</t>
+    </r>
+  </si>
+  <si>
     <t>4016</t>
   </si>
   <si>
@@ -5212,6 +6169,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/NRMC6JmvSFFHcMNm9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/6dvSYQ5LUK82UtyQ8</t>
+    </r>
+  </si>
+  <si>
     <t>4040</t>
   </si>
   <si>
@@ -5252,6 +6231,28 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/R1h5KXYWm7cNpuLT7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ce1ch7dgTAoa8eS99</t>
+    </r>
+  </si>
+  <si>
     <t>170</t>
   </si>
   <si>
@@ -5272,6 +6273,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/a8hDhn451US6ZJKg7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/BGtnkD9wFUFjmocR8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/H5EvCrzdfHc1s4RW6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/mFecJFq9tzP6VNcR8</t>
+    </r>
+  </si>
+  <si>
     <t>4079</t>
   </si>
   <si>
@@ -5312,6 +6357,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/8bw6R341ynynUv4w5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/AGVzgZPLMg5Khrg8A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/v677GYGfavVSaqs29</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/WrJri2Xpm25fdCBs7</t>
+    </r>
+  </si>
+  <si>
     <t>637</t>
   </si>
   <si>
@@ -5332,6 +6421,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/7Ga3AYBNncQXA35TA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/HMWefQZN3GThMjK16</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/mnbzF1kKHoATFqmh8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/PELtMYbJ4VcAxysC9</t>
+    </r>
+  </si>
+  <si>
     <t>648</t>
   </si>
   <si>
@@ -5352,6 +6485,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/firaP6nr2Z9RDbCX8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/endg7BJUZE383Ldo7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/XJaJkwwNkuNyxKdw9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/mzMwLmoaCpE7ZaWv9</t>
+    </r>
+  </si>
+  <si>
     <t>834</t>
   </si>
   <si>
@@ -5372,6 +6549,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/wMp9GHyejd3qKxJn7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/d2hk7tJGSZ52Yoan9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/kF3N6cStuvkajBpv5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/JwCfSa3cukU3Hcjq6</t>
+    </r>
+  </si>
+  <si>
     <t>738</t>
   </si>
   <si>
@@ -5392,6 +6613,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ig3TBVi1toXCtFjd9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/bnH4qomUk4TBmxkHA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5jj5uWuAhRFjHcxW8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/zNMSYRYv2SNsRsAT7</t>
+    </r>
+  </si>
+  <si>
     <t>355</t>
   </si>
   <si>
@@ -5412,6 +6677,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/6BitBhpGfwB3pMoQ8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5LqR3NoVdF6938cQA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/EoMEnssG9KRaPhtV7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ayGHikfeLMQEi7bS6</t>
+    </r>
+  </si>
+  <si>
     <t>363</t>
   </si>
   <si>
@@ -5432,6 +6741,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/yvYBmWAqAas9GQ7e8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/f3uUrzWRxG6s17rC8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/gwYNgqoNB1kjs6vs7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/L94X64ydjkVMknYD6</t>
+    </r>
+  </si>
+  <si>
     <t>776</t>
   </si>
   <si>
@@ -5452,6 +6805,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ocVnT59W8mgUWpXb9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/HGKsYrbgHF2ayee48</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/9SRR2tn1UGLu3RWj9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/roJ876eHfV4zm8wNA</t>
+    </r>
+  </si>
+  <si>
     <t>107</t>
   </si>
   <si>
@@ -5472,9 +6869,86 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/v76u7Y1J1Ah3ENuV7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/Yb5BMDdgtdYxGTxB7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/8BbJY6LXpKbQzMVdA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/oxKyF8fahfxedqgF8</t>
+    </r>
+  </si>
+  <si>
     <t>825</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/c9MQ22rnDgXkK6JA8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/fFs7EzcCfVDeNo9e6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/by4T44ZZkX8t2GQT7</t>
+    </r>
+  </si>
+  <si>
     <t>124</t>
   </si>
   <si>
@@ -5495,6 +6969,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/iKaCZdAFmcT32Q8s7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/qVU8LL3mKveW3ZPW6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/FpHjYFVJQM6YUevLA</t>
+    </r>
+  </si>
+  <si>
     <t>521</t>
   </si>
   <si>
@@ -5515,9 +7022,86 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/EvYtRfBRU7rbWhrZA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/PBEXL3ptu82zdTtt9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/hh8PZFMiajiEBDNi6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/ukxxLScnKgHYykYU9</t>
+    </r>
+  </si>
+  <si>
     <t>891</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/TgZdLynmEegdMKhD9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/6WPHDfofA4iU3UBh9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/3dRkw43X1wYuSUKG9</t>
+    </r>
+  </si>
+  <si>
     <t>206</t>
   </si>
   <si>
@@ -5538,6 +7122,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/4b5C1GKrMSDJ5dDi8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/UMHeTH8qM9nD4pne8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/WHTJAgza4Akop8GS9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/HUzUNs6LoY1bddet5</t>
+    </r>
+  </si>
+  <si>
     <t>125</t>
   </si>
   <si>
@@ -5558,6 +7186,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/sibKoAey5HWpCXuM9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/an1ZsoTPPHTu9HFKA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/7qhwJ9DpxQodnxaRA</t>
+    </r>
+  </si>
+  <si>
     <t>127</t>
   </si>
   <si>
@@ -5578,6 +7239,50 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/n19VqbzBeF9KJgfW6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/yAxUZUpCeGFT1Ehj6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/CdGzmfvr8fNLzZnj6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/zbTtfcd6Hqckytx3A</t>
+    </r>
+  </si>
+  <si>
     <t>530</t>
   </si>
   <si>
@@ -5598,6 +7303,39 @@
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/683aFsUn4uDTtxqW8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/7USBcXtzPJrBd7R8A</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/5erjFkQffpEj7b718</t>
+    </r>
+  </si>
+  <si>
     <t>576</t>
   </si>
   <si>
@@ -5615,6 +7353,50 @@
         <rFont val="Calibri"/>
       </rPr>
       <t>https://www.google.com/maps/place/SHOAL+CREEK+BLVD+%26+HANCOCK+DR,+Austin,+TX</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/8t12iujeT587qSm56</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/oAoDCHz7SMhhcSmo8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/GU4Q5b1gvgVXQ7gU6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="11"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>https://goo.gl/maps/2kurqLrzeM57gwKz8</t>
     </r>
   </si>
 </sst>
@@ -5772,7 +7554,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -5810,9 +7592,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10308,17 +12087,25 @@
         <f>HYPERLINK(G89)</f>
         <v>628</v>
       </c>
-      <c r="I89" s="13"/>
-      <c r="J89" s="13"/>
-      <c r="K89" s="13"/>
-      <c r="L89" s="13"/>
+      <c r="I89" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J89" t="s" s="12">
+        <v>629</v>
+      </c>
+      <c r="K89" t="s" s="12">
+        <v>630</v>
+      </c>
+      <c r="L89" t="s" s="12">
+        <v>631</v>
+      </c>
       <c r="M89" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="90" ht="133" customHeight="1">
       <c r="A90" t="s" s="3">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="B90" s="9">
         <v>5160817</v>
@@ -10327,28 +12114,36 @@
         <v>13</v>
       </c>
       <c r="D90" t="s" s="10">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="E90" s="11"/>
       <c r="F90" s="11"/>
       <c r="G90" t="s" s="12">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="H90" t="s" s="12">
         <f>HYPERLINK(G90)</f>
-        <v>632</v>
-      </c>
-      <c r="I90" s="13"/>
-      <c r="J90" s="13"/>
-      <c r="K90" s="13"/>
-      <c r="L90" s="13"/>
+        <v>635</v>
+      </c>
+      <c r="I90" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J90" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K90" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L90" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M90" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="91" ht="146" customHeight="1">
       <c r="A91" t="s" s="3">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="B91" s="9">
         <v>5156304</v>
@@ -10357,28 +12152,36 @@
         <v>13</v>
       </c>
       <c r="D91" t="s" s="10">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="E91" s="11"/>
       <c r="F91" s="11"/>
       <c r="G91" t="s" s="12">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="H91" t="s" s="12">
         <f>HYPERLINK(G91)</f>
-        <v>636</v>
-      </c>
-      <c r="I91" s="13"/>
-      <c r="J91" s="13"/>
-      <c r="K91" s="13"/>
-      <c r="L91" s="13"/>
+        <v>639</v>
+      </c>
+      <c r="I91" t="s" s="12">
+        <v>640</v>
+      </c>
+      <c r="J91" t="s" s="12">
+        <v>641</v>
+      </c>
+      <c r="K91" t="s" s="12">
+        <v>642</v>
+      </c>
+      <c r="L91" t="s" s="12">
+        <v>643</v>
+      </c>
       <c r="M91" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="92" ht="133" customHeight="1">
       <c r="A92" t="s" s="3">
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="B92" s="9">
         <v>0</v>
@@ -10387,28 +12190,36 @@
         <v>13</v>
       </c>
       <c r="D92" t="s" s="10">
-        <v>638</v>
+        <v>645</v>
       </c>
       <c r="E92" s="11"/>
       <c r="F92" s="11"/>
       <c r="G92" t="s" s="12">
-        <v>639</v>
+        <v>646</v>
       </c>
       <c r="H92" t="s" s="12">
         <f>HYPERLINK(G92)</f>
-        <v>640</v>
-      </c>
-      <c r="I92" s="13"/>
-      <c r="J92" s="13"/>
-      <c r="K92" s="13"/>
-      <c r="L92" s="13"/>
+        <v>647</v>
+      </c>
+      <c r="I92" t="s" s="12">
+        <v>648</v>
+      </c>
+      <c r="J92" t="s" s="12">
+        <v>649</v>
+      </c>
+      <c r="K92" t="s" s="12">
+        <v>650</v>
+      </c>
+      <c r="L92" t="s" s="12">
+        <v>651</v>
+      </c>
       <c r="M92" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="93" ht="159" customHeight="1">
       <c r="A93" t="s" s="3">
-        <v>641</v>
+        <v>652</v>
       </c>
       <c r="B93" s="9">
         <v>5164191</v>
@@ -10417,28 +12228,36 @@
         <v>13</v>
       </c>
       <c r="D93" t="s" s="10">
-        <v>642</v>
+        <v>653</v>
       </c>
       <c r="E93" s="11"/>
       <c r="F93" s="11"/>
       <c r="G93" t="s" s="12">
-        <v>643</v>
+        <v>654</v>
       </c>
       <c r="H93" t="s" s="12">
         <f>HYPERLINK(G93)</f>
-        <v>644</v>
-      </c>
-      <c r="I93" s="13"/>
-      <c r="J93" s="13"/>
-      <c r="K93" s="13"/>
-      <c r="L93" s="13"/>
+        <v>655</v>
+      </c>
+      <c r="I93" t="s" s="12">
+        <v>656</v>
+      </c>
+      <c r="J93" t="s" s="12">
+        <v>657</v>
+      </c>
+      <c r="K93" t="s" s="12">
+        <v>658</v>
+      </c>
+      <c r="L93" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M93" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="94" ht="146" customHeight="1">
       <c r="A94" t="s" s="3">
-        <v>645</v>
+        <v>659</v>
       </c>
       <c r="B94" s="9">
         <v>5148563</v>
@@ -10447,28 +12266,36 @@
         <v>13</v>
       </c>
       <c r="D94" t="s" s="10">
-        <v>646</v>
+        <v>660</v>
       </c>
       <c r="E94" s="11"/>
       <c r="F94" s="11"/>
       <c r="G94" t="s" s="12">
-        <v>647</v>
+        <v>661</v>
       </c>
       <c r="H94" t="s" s="12">
         <f>HYPERLINK(G94)</f>
-        <v>648</v>
-      </c>
-      <c r="I94" s="13"/>
-      <c r="J94" s="13"/>
-      <c r="K94" s="13"/>
-      <c r="L94" s="13"/>
+        <v>662</v>
+      </c>
+      <c r="I94" t="s" s="12">
+        <v>663</v>
+      </c>
+      <c r="J94" t="s" s="12">
+        <v>664</v>
+      </c>
+      <c r="K94" t="s" s="12">
+        <v>665</v>
+      </c>
+      <c r="L94" t="s" s="12">
+        <v>666</v>
+      </c>
       <c r="M94" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="95" ht="146" customHeight="1">
       <c r="A95" t="s" s="3">
-        <v>649</v>
+        <v>667</v>
       </c>
       <c r="B95" s="9">
         <v>5153874</v>
@@ -10477,28 +12304,36 @@
         <v>13</v>
       </c>
       <c r="D95" t="s" s="10">
-        <v>650</v>
+        <v>668</v>
       </c>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
       <c r="G95" t="s" s="12">
-        <v>651</v>
+        <v>669</v>
       </c>
       <c r="H95" t="s" s="12">
         <f>HYPERLINK(G95)</f>
-        <v>652</v>
-      </c>
-      <c r="I95" s="13"/>
-      <c r="J95" s="13"/>
-      <c r="K95" s="13"/>
-      <c r="L95" s="13"/>
+        <v>670</v>
+      </c>
+      <c r="I95" t="s" s="12">
+        <v>671</v>
+      </c>
+      <c r="J95" t="s" s="12">
+        <v>672</v>
+      </c>
+      <c r="K95" t="s" s="12">
+        <v>673</v>
+      </c>
+      <c r="L95" t="s" s="12">
+        <v>674</v>
+      </c>
       <c r="M95" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="96" ht="133" customHeight="1">
       <c r="A96" t="s" s="3">
-        <v>653</v>
+        <v>675</v>
       </c>
       <c r="B96" s="9">
         <v>5155597</v>
@@ -10507,28 +12342,36 @@
         <v>13</v>
       </c>
       <c r="D96" t="s" s="10">
-        <v>654</v>
+        <v>676</v>
       </c>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
       <c r="G96" t="s" s="12">
-        <v>655</v>
+        <v>677</v>
       </c>
       <c r="H96" t="s" s="12">
         <f>HYPERLINK(G96)</f>
-        <v>656</v>
-      </c>
-      <c r="I96" s="13"/>
-      <c r="J96" s="13"/>
-      <c r="K96" s="13"/>
-      <c r="L96" s="13"/>
+        <v>678</v>
+      </c>
+      <c r="I96" t="s" s="12">
+        <v>679</v>
+      </c>
+      <c r="J96" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K96" t="s" s="12">
+        <v>680</v>
+      </c>
+      <c r="L96" t="s" s="12">
+        <v>681</v>
+      </c>
       <c r="M96" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="97" ht="172" customHeight="1">
       <c r="A97" t="s" s="3">
-        <v>657</v>
+        <v>682</v>
       </c>
       <c r="B97" s="9">
         <v>5161612</v>
@@ -10537,28 +12380,36 @@
         <v>13</v>
       </c>
       <c r="D97" t="s" s="10">
-        <v>658</v>
+        <v>683</v>
       </c>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
       <c r="G97" t="s" s="12">
-        <v>659</v>
+        <v>684</v>
       </c>
       <c r="H97" t="s" s="12">
         <f>HYPERLINK(G97)</f>
-        <v>660</v>
-      </c>
-      <c r="I97" s="13"/>
-      <c r="J97" s="13"/>
-      <c r="K97" s="13"/>
-      <c r="L97" s="13"/>
+        <v>685</v>
+      </c>
+      <c r="I97" t="s" s="12">
+        <v>686</v>
+      </c>
+      <c r="J97" t="s" s="12">
+        <v>687</v>
+      </c>
+      <c r="K97" t="s" s="12">
+        <v>688</v>
+      </c>
+      <c r="L97" t="s" s="12">
+        <v>689</v>
+      </c>
       <c r="M97" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="98" ht="146" customHeight="1">
       <c r="A98" t="s" s="3">
-        <v>661</v>
+        <v>690</v>
       </c>
       <c r="B98" s="9">
         <v>5162805</v>
@@ -10567,28 +12418,36 @@
         <v>13</v>
       </c>
       <c r="D98" t="s" s="10">
-        <v>662</v>
+        <v>691</v>
       </c>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
       <c r="G98" t="s" s="12">
-        <v>663</v>
+        <v>692</v>
       </c>
       <c r="H98" t="s" s="12">
         <f>HYPERLINK(G98)</f>
-        <v>664</v>
-      </c>
-      <c r="I98" s="13"/>
-      <c r="J98" s="13"/>
-      <c r="K98" s="13"/>
-      <c r="L98" s="13"/>
+        <v>693</v>
+      </c>
+      <c r="I98" t="s" s="12">
+        <v>694</v>
+      </c>
+      <c r="J98" t="s" s="12">
+        <v>695</v>
+      </c>
+      <c r="K98" t="s" s="12">
+        <v>696</v>
+      </c>
+      <c r="L98" t="s" s="12">
+        <v>697</v>
+      </c>
       <c r="M98" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="99" ht="133" customHeight="1">
       <c r="A99" t="s" s="3">
-        <v>665</v>
+        <v>698</v>
       </c>
       <c r="B99" s="9">
         <v>0</v>
@@ -10597,28 +12456,36 @@
         <v>13</v>
       </c>
       <c r="D99" t="s" s="10">
-        <v>666</v>
+        <v>699</v>
       </c>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
       <c r="G99" t="s" s="12">
-        <v>667</v>
+        <v>700</v>
       </c>
       <c r="H99" t="s" s="12">
         <f>HYPERLINK(G99)</f>
-        <v>668</v>
-      </c>
-      <c r="I99" s="13"/>
-      <c r="J99" s="13"/>
-      <c r="K99" s="13"/>
-      <c r="L99" s="13"/>
+        <v>701</v>
+      </c>
+      <c r="I99" t="s" s="12">
+        <v>702</v>
+      </c>
+      <c r="J99" t="s" s="12">
+        <v>703</v>
+      </c>
+      <c r="K99" t="s" s="12">
+        <v>696</v>
+      </c>
+      <c r="L99" t="s" s="12">
+        <v>704</v>
+      </c>
       <c r="M99" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="100" ht="172" customHeight="1">
       <c r="A100" t="s" s="3">
-        <v>669</v>
+        <v>705</v>
       </c>
       <c r="B100" s="9">
         <v>5155501</v>
@@ -10627,28 +12494,36 @@
         <v>13</v>
       </c>
       <c r="D100" t="s" s="10">
-        <v>670</v>
+        <v>706</v>
       </c>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
       <c r="G100" t="s" s="12">
-        <v>671</v>
+        <v>707</v>
       </c>
       <c r="H100" t="s" s="12">
         <f>HYPERLINK(G100)</f>
-        <v>672</v>
-      </c>
-      <c r="I100" s="13"/>
-      <c r="J100" s="13"/>
-      <c r="K100" s="13"/>
-      <c r="L100" s="13"/>
+        <v>708</v>
+      </c>
+      <c r="I100" t="s" s="12">
+        <v>709</v>
+      </c>
+      <c r="J100" t="s" s="12">
+        <v>710</v>
+      </c>
+      <c r="K100" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L100" t="s" s="12">
+        <v>711</v>
+      </c>
       <c r="M100" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="101" ht="159" customHeight="1">
       <c r="A101" t="s" s="3">
-        <v>673</v>
+        <v>712</v>
       </c>
       <c r="B101" s="9">
         <v>5160656</v>
@@ -10657,28 +12532,36 @@
         <v>13</v>
       </c>
       <c r="D101" t="s" s="10">
-        <v>674</v>
+        <v>713</v>
       </c>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
       <c r="G101" t="s" s="12">
-        <v>675</v>
+        <v>714</v>
       </c>
       <c r="H101" t="s" s="12">
         <f>HYPERLINK(G101)</f>
-        <v>676</v>
-      </c>
-      <c r="I101" s="13"/>
-      <c r="J101" s="13"/>
-      <c r="K101" s="13"/>
-      <c r="L101" s="13"/>
+        <v>715</v>
+      </c>
+      <c r="I101" t="s" s="12">
+        <v>716</v>
+      </c>
+      <c r="J101" t="s" s="12">
+        <v>717</v>
+      </c>
+      <c r="K101" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L101" t="s" s="12">
+        <v>718</v>
+      </c>
       <c r="M101" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="102" ht="133" customHeight="1">
       <c r="A102" t="s" s="3">
-        <v>677</v>
+        <v>719</v>
       </c>
       <c r="B102" s="9">
         <v>5154206</v>
@@ -10687,28 +12570,36 @@
         <v>13</v>
       </c>
       <c r="D102" t="s" s="10">
-        <v>678</v>
+        <v>720</v>
       </c>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
       <c r="G102" t="s" s="12">
-        <v>679</v>
+        <v>721</v>
       </c>
       <c r="H102" t="s" s="12">
         <f>HYPERLINK(G102)</f>
-        <v>680</v>
-      </c>
-      <c r="I102" s="13"/>
-      <c r="J102" s="13"/>
-      <c r="K102" s="13"/>
-      <c r="L102" s="13"/>
+        <v>722</v>
+      </c>
+      <c r="I102" t="s" s="12">
+        <v>723</v>
+      </c>
+      <c r="J102" t="s" s="12">
+        <v>724</v>
+      </c>
+      <c r="K102" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L102" t="s" s="12">
+        <v>725</v>
+      </c>
       <c r="M102" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="103" ht="146" customHeight="1">
       <c r="A103" t="s" s="3">
-        <v>681</v>
+        <v>726</v>
       </c>
       <c r="B103" s="9">
         <v>5154815</v>
@@ -10717,28 +12608,36 @@
         <v>13</v>
       </c>
       <c r="D103" t="s" s="10">
-        <v>682</v>
+        <v>727</v>
       </c>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
       <c r="G103" t="s" s="12">
-        <v>683</v>
+        <v>728</v>
       </c>
       <c r="H103" t="s" s="12">
         <f>HYPERLINK(G103)</f>
-        <v>684</v>
-      </c>
-      <c r="I103" s="13"/>
-      <c r="J103" s="13"/>
-      <c r="K103" s="13"/>
-      <c r="L103" s="13"/>
+        <v>729</v>
+      </c>
+      <c r="I103" t="s" s="12">
+        <v>730</v>
+      </c>
+      <c r="J103" t="s" s="12">
+        <v>731</v>
+      </c>
+      <c r="K103" t="s" s="12">
+        <v>732</v>
+      </c>
+      <c r="L103" t="s" s="12">
+        <v>733</v>
+      </c>
       <c r="M103" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="104" ht="172" customHeight="1">
       <c r="A104" t="s" s="3">
-        <v>685</v>
+        <v>734</v>
       </c>
       <c r="B104" s="9">
         <v>5144930</v>
@@ -10747,28 +12646,36 @@
         <v>13</v>
       </c>
       <c r="D104" t="s" s="10">
-        <v>686</v>
+        <v>735</v>
       </c>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
       <c r="G104" t="s" s="12">
-        <v>687</v>
+        <v>736</v>
       </c>
       <c r="H104" t="s" s="12">
         <f>HYPERLINK(G104)</f>
-        <v>688</v>
-      </c>
-      <c r="I104" s="13"/>
-      <c r="J104" s="13"/>
-      <c r="K104" s="13"/>
-      <c r="L104" s="13"/>
+        <v>737</v>
+      </c>
+      <c r="I104" t="s" s="12">
+        <v>738</v>
+      </c>
+      <c r="J104" t="s" s="12">
+        <v>739</v>
+      </c>
+      <c r="K104" t="s" s="12">
+        <v>740</v>
+      </c>
+      <c r="L104" t="s" s="12">
+        <v>741</v>
+      </c>
       <c r="M104" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="105" ht="159" customHeight="1">
       <c r="A105" t="s" s="3">
-        <v>689</v>
+        <v>742</v>
       </c>
       <c r="B105" s="9">
         <v>5148691</v>
@@ -10777,28 +12684,36 @@
         <v>13</v>
       </c>
       <c r="D105" t="s" s="10">
-        <v>690</v>
+        <v>743</v>
       </c>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
       <c r="G105" t="s" s="12">
-        <v>691</v>
+        <v>744</v>
       </c>
       <c r="H105" t="s" s="12">
         <f>HYPERLINK(G105)</f>
-        <v>692</v>
-      </c>
-      <c r="I105" s="13"/>
-      <c r="J105" s="13"/>
-      <c r="K105" s="13"/>
-      <c r="L105" s="13"/>
+        <v>745</v>
+      </c>
+      <c r="I105" t="s" s="12">
+        <v>746</v>
+      </c>
+      <c r="J105" t="s" s="12">
+        <v>747</v>
+      </c>
+      <c r="K105" t="s" s="12">
+        <v>748</v>
+      </c>
+      <c r="L105" t="s" s="12">
+        <v>749</v>
+      </c>
       <c r="M105" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="106" ht="133" customHeight="1">
       <c r="A106" t="s" s="3">
-        <v>693</v>
+        <v>750</v>
       </c>
       <c r="B106" s="9">
         <v>5160982</v>
@@ -10807,28 +12722,36 @@
         <v>13</v>
       </c>
       <c r="D106" t="s" s="10">
-        <v>694</v>
+        <v>751</v>
       </c>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
       <c r="G106" t="s" s="12">
-        <v>695</v>
+        <v>752</v>
       </c>
       <c r="H106" t="s" s="12">
         <f>HYPERLINK(G106)</f>
-        <v>696</v>
-      </c>
-      <c r="I106" s="13"/>
-      <c r="J106" s="13"/>
-      <c r="K106" s="13"/>
-      <c r="L106" s="13"/>
+        <v>753</v>
+      </c>
+      <c r="I106" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J106" t="s" s="12">
+        <v>754</v>
+      </c>
+      <c r="K106" t="s" s="12">
+        <v>755</v>
+      </c>
+      <c r="L106" t="s" s="12">
+        <v>756</v>
+      </c>
       <c r="M106" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="107" ht="159" customHeight="1">
       <c r="A107" t="s" s="3">
-        <v>697</v>
+        <v>757</v>
       </c>
       <c r="B107" s="9">
         <v>5144899</v>
@@ -10837,28 +12760,36 @@
         <v>13</v>
       </c>
       <c r="D107" t="s" s="10">
-        <v>698</v>
+        <v>758</v>
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
       <c r="G107" t="s" s="12">
-        <v>699</v>
+        <v>759</v>
       </c>
       <c r="H107" t="s" s="12">
         <f>HYPERLINK(G107)</f>
-        <v>700</v>
-      </c>
-      <c r="I107" s="13"/>
-      <c r="J107" s="13"/>
-      <c r="K107" s="13"/>
-      <c r="L107" s="13"/>
+        <v>760</v>
+      </c>
+      <c r="I107" t="s" s="12">
+        <v>761</v>
+      </c>
+      <c r="J107" t="s" s="12">
+        <v>762</v>
+      </c>
+      <c r="K107" t="s" s="12">
+        <v>763</v>
+      </c>
+      <c r="L107" t="s" s="12">
+        <v>764</v>
+      </c>
       <c r="M107" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="108" ht="172" customHeight="1">
       <c r="A108" t="s" s="3">
-        <v>701</v>
+        <v>765</v>
       </c>
       <c r="B108" s="9">
         <v>5147043</v>
@@ -10867,28 +12798,36 @@
         <v>13</v>
       </c>
       <c r="D108" t="s" s="10">
-        <v>702</v>
+        <v>766</v>
       </c>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
       <c r="G108" t="s" s="12">
-        <v>703</v>
+        <v>767</v>
       </c>
       <c r="H108" t="s" s="12">
         <f>HYPERLINK(G108)</f>
-        <v>704</v>
-      </c>
-      <c r="I108" s="13"/>
-      <c r="J108" s="13"/>
-      <c r="K108" s="13"/>
-      <c r="L108" s="13"/>
+        <v>768</v>
+      </c>
+      <c r="I108" t="s" s="12">
+        <v>769</v>
+      </c>
+      <c r="J108" t="s" s="12">
+        <v>770</v>
+      </c>
+      <c r="K108" t="s" s="12">
+        <v>771</v>
+      </c>
+      <c r="L108" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M108" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="109" ht="172" customHeight="1">
       <c r="A109" t="s" s="3">
-        <v>705</v>
+        <v>772</v>
       </c>
       <c r="B109" s="9">
         <v>5148485</v>
@@ -10908,17 +12847,25 @@
         <f>HYPERLINK(G109)</f>
         <v>577</v>
       </c>
-      <c r="I109" s="13"/>
-      <c r="J109" s="13"/>
-      <c r="K109" s="13"/>
-      <c r="L109" s="13"/>
+      <c r="I109" t="s" s="12">
+        <v>773</v>
+      </c>
+      <c r="J109" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K109" t="s" s="12">
+        <v>774</v>
+      </c>
+      <c r="L109" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M109" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="110" ht="172" customHeight="1">
       <c r="A110" t="s" s="3">
-        <v>706</v>
+        <v>775</v>
       </c>
       <c r="B110" s="9">
         <v>5148415</v>
@@ -10938,17 +12885,25 @@
         <f>HYPERLINK(G110)</f>
         <v>577</v>
       </c>
-      <c r="I110" s="13"/>
-      <c r="J110" s="13"/>
-      <c r="K110" s="13"/>
-      <c r="L110" s="13"/>
+      <c r="I110" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J110" t="s" s="12">
+        <v>776</v>
+      </c>
+      <c r="K110" t="s" s="12">
+        <v>777</v>
+      </c>
+      <c r="L110" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M110" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="111" ht="159" customHeight="1">
       <c r="A111" t="s" s="3">
-        <v>707</v>
+        <v>778</v>
       </c>
       <c r="B111" s="9">
         <v>5148537</v>
@@ -10968,17 +12923,25 @@
         <f>HYPERLINK(G111)</f>
         <v>586</v>
       </c>
-      <c r="I111" s="13"/>
-      <c r="J111" s="13"/>
-      <c r="K111" s="13"/>
-      <c r="L111" s="13"/>
+      <c r="I111" t="s" s="12">
+        <v>779</v>
+      </c>
+      <c r="J111" t="s" s="12">
+        <v>780</v>
+      </c>
+      <c r="K111" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L111" t="s" s="12">
+        <v>781</v>
+      </c>
       <c r="M111" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="112" ht="185" customHeight="1">
       <c r="A112" t="s" s="3">
-        <v>708</v>
+        <v>782</v>
       </c>
       <c r="B112" s="9">
         <v>5162491</v>
@@ -10987,28 +12950,36 @@
         <v>13</v>
       </c>
       <c r="D112" t="s" s="10">
-        <v>709</v>
+        <v>783</v>
       </c>
       <c r="E112" s="11"/>
       <c r="F112" s="11"/>
       <c r="G112" t="s" s="12">
-        <v>710</v>
+        <v>784</v>
       </c>
       <c r="H112" t="s" s="12">
         <f>HYPERLINK(G112)</f>
-        <v>711</v>
-      </c>
-      <c r="I112" s="13"/>
-      <c r="J112" s="13"/>
-      <c r="K112" s="13"/>
-      <c r="L112" s="13"/>
+        <v>785</v>
+      </c>
+      <c r="I112" t="s" s="12">
+        <v>786</v>
+      </c>
+      <c r="J112" t="s" s="12">
+        <v>787</v>
+      </c>
+      <c r="K112" t="s" s="12">
+        <v>788</v>
+      </c>
+      <c r="L112" t="s" s="12">
+        <v>789</v>
+      </c>
       <c r="M112" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="113" ht="159" customHeight="1">
       <c r="A113" t="s" s="3">
-        <v>712</v>
+        <v>790</v>
       </c>
       <c r="B113" s="9">
         <v>5166976</v>
@@ -11017,28 +12988,36 @@
         <v>13</v>
       </c>
       <c r="D113" t="s" s="10">
-        <v>713</v>
+        <v>791</v>
       </c>
       <c r="E113" s="11"/>
       <c r="F113" s="11"/>
       <c r="G113" t="s" s="12">
-        <v>714</v>
+        <v>792</v>
       </c>
       <c r="H113" t="s" s="12">
         <f>HYPERLINK(G113)</f>
-        <v>715</v>
-      </c>
-      <c r="I113" s="13"/>
-      <c r="J113" s="13"/>
-      <c r="K113" s="13"/>
-      <c r="L113" s="13"/>
+        <v>793</v>
+      </c>
+      <c r="I113" t="s" s="12">
+        <v>794</v>
+      </c>
+      <c r="J113" t="s" s="12">
+        <v>795</v>
+      </c>
+      <c r="K113" t="s" s="12">
+        <v>796</v>
+      </c>
+      <c r="L113" t="s" s="12">
+        <v>797</v>
+      </c>
       <c r="M113" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="114" ht="185" customHeight="1">
       <c r="A114" t="s" s="3">
-        <v>716</v>
+        <v>798</v>
       </c>
       <c r="B114" s="9">
         <v>5145942</v>
@@ -11058,17 +13037,25 @@
         <f>HYPERLINK(G114)</f>
         <v>322</v>
       </c>
-      <c r="I114" s="13"/>
-      <c r="J114" s="13"/>
-      <c r="K114" s="13"/>
-      <c r="L114" s="13"/>
+      <c r="I114" t="s" s="12">
+        <v>799</v>
+      </c>
+      <c r="J114" t="s" s="12">
+        <v>800</v>
+      </c>
+      <c r="K114" t="s" s="12">
+        <v>801</v>
+      </c>
+      <c r="L114" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M114" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="115" ht="172" customHeight="1">
       <c r="A115" t="s" s="3">
-        <v>717</v>
+        <v>802</v>
       </c>
       <c r="B115" s="9">
         <v>5145318</v>
@@ -11077,28 +13064,36 @@
         <v>13</v>
       </c>
       <c r="D115" t="s" s="10">
-        <v>718</v>
+        <v>803</v>
       </c>
       <c r="E115" s="11"/>
       <c r="F115" s="11"/>
       <c r="G115" t="s" s="12">
-        <v>719</v>
+        <v>804</v>
       </c>
       <c r="H115" t="s" s="12">
         <f>HYPERLINK(G115)</f>
-        <v>720</v>
-      </c>
-      <c r="I115" s="13"/>
-      <c r="J115" s="13"/>
-      <c r="K115" s="13"/>
-      <c r="L115" s="13"/>
+        <v>805</v>
+      </c>
+      <c r="I115" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J115" t="s" s="12">
+        <v>806</v>
+      </c>
+      <c r="K115" t="s" s="12">
+        <v>807</v>
+      </c>
+      <c r="L115" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M115" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="116" ht="133" customHeight="1">
       <c r="A116" t="s" s="3">
-        <v>721</v>
+        <v>808</v>
       </c>
       <c r="B116" s="9">
         <v>5160920</v>
@@ -11107,28 +13102,36 @@
         <v>13</v>
       </c>
       <c r="D116" t="s" s="10">
-        <v>722</v>
+        <v>809</v>
       </c>
       <c r="E116" s="11"/>
       <c r="F116" s="11"/>
       <c r="G116" t="s" s="12">
-        <v>723</v>
+        <v>810</v>
       </c>
       <c r="H116" t="s" s="12">
         <f>HYPERLINK(G116)</f>
-        <v>724</v>
-      </c>
-      <c r="I116" s="13"/>
-      <c r="J116" s="13"/>
-      <c r="K116" s="13"/>
-      <c r="L116" s="13"/>
+        <v>811</v>
+      </c>
+      <c r="I116" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J116" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K116" t="s" s="12">
+        <v>812</v>
+      </c>
+      <c r="L116" t="s" s="12">
+        <v>813</v>
+      </c>
       <c r="M116" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="117" ht="133" customHeight="1">
       <c r="A117" t="s" s="3">
-        <v>725</v>
+        <v>814</v>
       </c>
       <c r="B117" s="9">
         <v>5153243</v>
@@ -11137,28 +13140,36 @@
         <v>13</v>
       </c>
       <c r="D117" t="s" s="10">
-        <v>726</v>
+        <v>815</v>
       </c>
       <c r="E117" s="11"/>
       <c r="F117" s="11"/>
       <c r="G117" t="s" s="12">
-        <v>727</v>
+        <v>816</v>
       </c>
       <c r="H117" t="s" s="12">
         <f>HYPERLINK(G117)</f>
-        <v>728</v>
-      </c>
-      <c r="I117" s="13"/>
-      <c r="J117" s="13"/>
-      <c r="K117" s="13"/>
-      <c r="L117" s="13"/>
+        <v>817</v>
+      </c>
+      <c r="I117" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J117" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K117" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L117" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M117" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="118" ht="146" customHeight="1">
       <c r="A118" t="s" s="3">
-        <v>729</v>
+        <v>818</v>
       </c>
       <c r="B118" s="9">
         <v>5152271</v>
@@ -11167,28 +13178,36 @@
         <v>13</v>
       </c>
       <c r="D118" t="s" s="10">
-        <v>730</v>
+        <v>819</v>
       </c>
       <c r="E118" s="11"/>
       <c r="F118" s="11"/>
       <c r="G118" t="s" s="12">
-        <v>731</v>
+        <v>820</v>
       </c>
       <c r="H118" t="s" s="12">
         <f>HYPERLINK(G118)</f>
-        <v>732</v>
-      </c>
-      <c r="I118" s="13"/>
-      <c r="J118" s="13"/>
-      <c r="K118" s="13"/>
-      <c r="L118" s="13"/>
+        <v>821</v>
+      </c>
+      <c r="I118" t="s" s="12">
+        <v>822</v>
+      </c>
+      <c r="J118" t="s" s="12">
+        <v>823</v>
+      </c>
+      <c r="K118" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L118" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M118" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="119" ht="146" customHeight="1">
       <c r="A119" t="s" s="3">
-        <v>733</v>
+        <v>824</v>
       </c>
       <c r="B119" s="9">
         <v>5160367</v>
@@ -11197,28 +13216,36 @@
         <v>13</v>
       </c>
       <c r="D119" t="s" s="10">
-        <v>734</v>
+        <v>825</v>
       </c>
       <c r="E119" s="11"/>
       <c r="F119" s="11"/>
       <c r="G119" t="s" s="12">
-        <v>735</v>
+        <v>826</v>
       </c>
       <c r="H119" t="s" s="12">
         <f>HYPERLINK(G119)</f>
-        <v>736</v>
-      </c>
-      <c r="I119" s="13"/>
-      <c r="J119" s="13"/>
-      <c r="K119" s="13"/>
-      <c r="L119" s="13"/>
+        <v>827</v>
+      </c>
+      <c r="I119" t="s" s="12">
+        <v>828</v>
+      </c>
+      <c r="J119" t="s" s="12">
+        <v>829</v>
+      </c>
+      <c r="K119" t="s" s="12">
+        <v>830</v>
+      </c>
+      <c r="L119" t="s" s="12">
+        <v>831</v>
+      </c>
       <c r="M119" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="120" ht="172" customHeight="1">
       <c r="A120" t="s" s="3">
-        <v>737</v>
+        <v>832</v>
       </c>
       <c r="B120" s="9">
         <v>5161260</v>
@@ -11227,28 +13254,36 @@
         <v>13</v>
       </c>
       <c r="D120" t="s" s="10">
-        <v>738</v>
+        <v>833</v>
       </c>
       <c r="E120" s="11"/>
       <c r="F120" s="11"/>
       <c r="G120" t="s" s="12">
-        <v>739</v>
+        <v>834</v>
       </c>
       <c r="H120" t="s" s="12">
         <f>HYPERLINK(G120)</f>
-        <v>740</v>
-      </c>
-      <c r="I120" s="13"/>
-      <c r="J120" s="13"/>
-      <c r="K120" s="13"/>
-      <c r="L120" s="13"/>
+        <v>835</v>
+      </c>
+      <c r="I120" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="J120" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K120" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L120" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M120" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="121" ht="146" customHeight="1">
       <c r="A121" t="s" s="3">
-        <v>741</v>
+        <v>836</v>
       </c>
       <c r="B121" s="9">
         <v>5160691</v>
@@ -11257,28 +13292,36 @@
         <v>13</v>
       </c>
       <c r="D121" t="s" s="10">
-        <v>742</v>
+        <v>837</v>
       </c>
       <c r="E121" s="11"/>
       <c r="F121" s="11"/>
       <c r="G121" t="s" s="12">
-        <v>743</v>
+        <v>838</v>
       </c>
       <c r="H121" t="s" s="12">
         <f>HYPERLINK(G121)</f>
-        <v>744</v>
-      </c>
-      <c r="I121" s="13"/>
-      <c r="J121" s="13"/>
-      <c r="K121" s="13"/>
-      <c r="L121" s="13"/>
+        <v>839</v>
+      </c>
+      <c r="I121" t="s" s="12">
+        <v>840</v>
+      </c>
+      <c r="J121" t="s" s="12">
+        <v>841</v>
+      </c>
+      <c r="K121" t="s" s="12">
+        <v>842</v>
+      </c>
+      <c r="L121" t="s" s="12">
+        <v>843</v>
+      </c>
       <c r="M121" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="122" ht="185" customHeight="1">
       <c r="A122" t="s" s="3">
-        <v>745</v>
+        <v>844</v>
       </c>
       <c r="B122" s="9">
         <v>5164054</v>
@@ -11287,28 +13330,36 @@
         <v>13</v>
       </c>
       <c r="D122" t="s" s="10">
-        <v>746</v>
+        <v>845</v>
       </c>
       <c r="E122" s="11"/>
       <c r="F122" s="11"/>
       <c r="G122" t="s" s="12">
-        <v>747</v>
+        <v>846</v>
       </c>
       <c r="H122" t="s" s="12">
         <f>HYPERLINK(G122)</f>
-        <v>748</v>
-      </c>
-      <c r="I122" s="13"/>
-      <c r="J122" s="13"/>
-      <c r="K122" s="13"/>
-      <c r="L122" s="13"/>
+        <v>847</v>
+      </c>
+      <c r="I122" t="s" s="12">
+        <v>848</v>
+      </c>
+      <c r="J122" t="s" s="12">
+        <v>849</v>
+      </c>
+      <c r="K122" t="s" s="12">
+        <v>850</v>
+      </c>
+      <c r="L122" t="s" s="12">
+        <v>851</v>
+      </c>
       <c r="M122" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="123" ht="146" customHeight="1">
       <c r="A123" t="s" s="3">
-        <v>749</v>
+        <v>852</v>
       </c>
       <c r="B123" s="9">
         <v>5164505</v>
@@ -11317,28 +13368,36 @@
         <v>13</v>
       </c>
       <c r="D123" t="s" s="10">
-        <v>750</v>
+        <v>853</v>
       </c>
       <c r="E123" s="11"/>
       <c r="F123" s="11"/>
       <c r="G123" t="s" s="12">
-        <v>751</v>
+        <v>854</v>
       </c>
       <c r="H123" t="s" s="12">
         <f>HYPERLINK(G123)</f>
-        <v>752</v>
-      </c>
-      <c r="I123" s="13"/>
-      <c r="J123" s="13"/>
-      <c r="K123" s="13"/>
-      <c r="L123" s="13"/>
+        <v>855</v>
+      </c>
+      <c r="I123" t="s" s="12">
+        <v>856</v>
+      </c>
+      <c r="J123" t="s" s="12">
+        <v>857</v>
+      </c>
+      <c r="K123" t="s" s="12">
+        <v>858</v>
+      </c>
+      <c r="L123" t="s" s="12">
+        <v>859</v>
+      </c>
       <c r="M123" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="124" ht="172" customHeight="1">
       <c r="A124" t="s" s="3">
-        <v>753</v>
+        <v>860</v>
       </c>
       <c r="B124" s="9">
         <v>5165251</v>
@@ -11347,28 +13406,36 @@
         <v>13</v>
       </c>
       <c r="D124" t="s" s="10">
-        <v>754</v>
+        <v>861</v>
       </c>
       <c r="E124" s="11"/>
       <c r="F124" s="11"/>
       <c r="G124" t="s" s="12">
-        <v>755</v>
+        <v>862</v>
       </c>
       <c r="H124" t="s" s="12">
         <f>HYPERLINK(G124)</f>
-        <v>756</v>
-      </c>
-      <c r="I124" s="13"/>
-      <c r="J124" s="13"/>
-      <c r="K124" s="13"/>
-      <c r="L124" s="13"/>
+        <v>863</v>
+      </c>
+      <c r="I124" t="s" s="12">
+        <v>864</v>
+      </c>
+      <c r="J124" t="s" s="12">
+        <v>865</v>
+      </c>
+      <c r="K124" t="s" s="12">
+        <v>866</v>
+      </c>
+      <c r="L124" t="s" s="12">
+        <v>867</v>
+      </c>
       <c r="M124" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="125" ht="159" customHeight="1">
       <c r="A125" t="s" s="3">
-        <v>757</v>
+        <v>868</v>
       </c>
       <c r="B125" s="9">
         <v>5156211</v>
@@ -11377,28 +13444,36 @@
         <v>13</v>
       </c>
       <c r="D125" t="s" s="10">
-        <v>758</v>
+        <v>869</v>
       </c>
       <c r="E125" s="11"/>
       <c r="F125" s="11"/>
       <c r="G125" t="s" s="12">
-        <v>759</v>
+        <v>870</v>
       </c>
       <c r="H125" t="s" s="12">
         <f>HYPERLINK(G125)</f>
-        <v>760</v>
-      </c>
-      <c r="I125" s="13"/>
-      <c r="J125" s="13"/>
-      <c r="K125" s="13"/>
-      <c r="L125" s="13"/>
+        <v>871</v>
+      </c>
+      <c r="I125" t="s" s="12">
+        <v>872</v>
+      </c>
+      <c r="J125" t="s" s="12">
+        <v>873</v>
+      </c>
+      <c r="K125" t="s" s="12">
+        <v>874</v>
+      </c>
+      <c r="L125" t="s" s="12">
+        <v>875</v>
+      </c>
       <c r="M125" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="126" ht="146" customHeight="1">
       <c r="A126" t="s" s="3">
-        <v>761</v>
+        <v>876</v>
       </c>
       <c r="B126" s="9">
         <v>5161138</v>
@@ -11407,28 +13482,36 @@
         <v>13</v>
       </c>
       <c r="D126" t="s" s="10">
-        <v>762</v>
+        <v>877</v>
       </c>
       <c r="E126" s="11"/>
       <c r="F126" s="11"/>
       <c r="G126" t="s" s="12">
-        <v>763</v>
+        <v>878</v>
       </c>
       <c r="H126" t="s" s="12">
         <f>HYPERLINK(G126)</f>
-        <v>764</v>
-      </c>
-      <c r="I126" s="13"/>
-      <c r="J126" s="13"/>
-      <c r="K126" s="13"/>
-      <c r="L126" s="13"/>
+        <v>879</v>
+      </c>
+      <c r="I126" t="s" s="12">
+        <v>880</v>
+      </c>
+      <c r="J126" t="s" s="12">
+        <v>881</v>
+      </c>
+      <c r="K126" t="s" s="12">
+        <v>882</v>
+      </c>
+      <c r="L126" t="s" s="12">
+        <v>883</v>
+      </c>
       <c r="M126" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="127" ht="146" customHeight="1">
       <c r="A127" t="s" s="3">
-        <v>765</v>
+        <v>884</v>
       </c>
       <c r="B127" s="9">
         <v>5159056</v>
@@ -11437,28 +13520,36 @@
         <v>13</v>
       </c>
       <c r="D127" t="s" s="10">
-        <v>766</v>
+        <v>885</v>
       </c>
       <c r="E127" s="11"/>
       <c r="F127" s="11"/>
       <c r="G127" t="s" s="12">
-        <v>767</v>
+        <v>886</v>
       </c>
       <c r="H127" t="s" s="12">
         <f>HYPERLINK(G127)</f>
-        <v>768</v>
-      </c>
-      <c r="I127" s="13"/>
-      <c r="J127" s="13"/>
-      <c r="K127" s="13"/>
-      <c r="L127" s="13"/>
+        <v>887</v>
+      </c>
+      <c r="I127" t="s" s="12">
+        <v>888</v>
+      </c>
+      <c r="J127" t="s" s="12">
+        <v>889</v>
+      </c>
+      <c r="K127" t="s" s="12">
+        <v>890</v>
+      </c>
+      <c r="L127" t="s" s="12">
+        <v>891</v>
+      </c>
       <c r="M127" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="128" ht="146" customHeight="1">
       <c r="A128" t="s" s="3">
-        <v>769</v>
+        <v>892</v>
       </c>
       <c r="B128" s="9">
         <v>5152967</v>
@@ -11467,28 +13558,36 @@
         <v>13</v>
       </c>
       <c r="D128" t="s" s="10">
-        <v>770</v>
+        <v>893</v>
       </c>
       <c r="E128" s="11"/>
       <c r="F128" s="11"/>
       <c r="G128" t="s" s="12">
-        <v>771</v>
+        <v>894</v>
       </c>
       <c r="H128" t="s" s="12">
         <f>HYPERLINK(G128)</f>
-        <v>772</v>
-      </c>
-      <c r="I128" s="13"/>
-      <c r="J128" s="13"/>
-      <c r="K128" s="13"/>
-      <c r="L128" s="13"/>
+        <v>895</v>
+      </c>
+      <c r="I128" t="s" s="12">
+        <v>896</v>
+      </c>
+      <c r="J128" t="s" s="12">
+        <v>897</v>
+      </c>
+      <c r="K128" t="s" s="12">
+        <v>898</v>
+      </c>
+      <c r="L128" t="s" s="12">
+        <v>899</v>
+      </c>
       <c r="M128" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="129" ht="133" customHeight="1">
       <c r="A129" t="s" s="3">
-        <v>773</v>
+        <v>900</v>
       </c>
       <c r="B129" s="9">
         <v>5154965</v>
@@ -11497,28 +13596,36 @@
         <v>13</v>
       </c>
       <c r="D129" t="s" s="10">
-        <v>774</v>
+        <v>901</v>
       </c>
       <c r="E129" s="11"/>
       <c r="F129" s="11"/>
       <c r="G129" t="s" s="12">
-        <v>775</v>
+        <v>902</v>
       </c>
       <c r="H129" t="s" s="12">
         <f>HYPERLINK(G129)</f>
-        <v>776</v>
-      </c>
-      <c r="I129" s="13"/>
-      <c r="J129" s="13"/>
-      <c r="K129" s="13"/>
-      <c r="L129" s="13"/>
+        <v>903</v>
+      </c>
+      <c r="I129" t="s" s="12">
+        <v>904</v>
+      </c>
+      <c r="J129" t="s" s="12">
+        <v>905</v>
+      </c>
+      <c r="K129" t="s" s="12">
+        <v>906</v>
+      </c>
+      <c r="L129" t="s" s="12">
+        <v>907</v>
+      </c>
       <c r="M129" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="130" ht="146" customHeight="1">
       <c r="A130" t="s" s="3">
-        <v>777</v>
+        <v>908</v>
       </c>
       <c r="B130" s="9">
         <v>5153256</v>
@@ -11538,17 +13645,25 @@
         <f>HYPERLINK(G130)</f>
         <v>188</v>
       </c>
-      <c r="I130" s="13"/>
-      <c r="J130" s="13"/>
-      <c r="K130" s="13"/>
-      <c r="L130" s="13"/>
+      <c r="I130" t="s" s="12">
+        <v>909</v>
+      </c>
+      <c r="J130" t="s" s="12">
+        <v>910</v>
+      </c>
+      <c r="K130" t="s" s="12">
+        <v>911</v>
+      </c>
+      <c r="L130" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M130" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="131" ht="159" customHeight="1">
       <c r="A131" t="s" s="3">
-        <v>778</v>
+        <v>912</v>
       </c>
       <c r="B131" s="9">
         <v>5152555</v>
@@ -11557,28 +13672,36 @@
         <v>13</v>
       </c>
       <c r="D131" t="s" s="10">
-        <v>779</v>
+        <v>913</v>
       </c>
       <c r="E131" s="11"/>
       <c r="F131" s="11"/>
       <c r="G131" t="s" s="12">
-        <v>780</v>
+        <v>914</v>
       </c>
       <c r="H131" t="s" s="12">
         <f>HYPERLINK(G131)</f>
-        <v>781</v>
-      </c>
-      <c r="I131" s="13"/>
-      <c r="J131" s="13"/>
-      <c r="K131" s="13"/>
-      <c r="L131" s="13"/>
+        <v>915</v>
+      </c>
+      <c r="I131" t="s" s="12">
+        <v>916</v>
+      </c>
+      <c r="J131" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K131" t="s" s="12">
+        <v>917</v>
+      </c>
+      <c r="L131" t="s" s="12">
+        <v>918</v>
+      </c>
       <c r="M131" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="132" ht="159" customHeight="1">
       <c r="A132" t="s" s="3">
-        <v>782</v>
+        <v>919</v>
       </c>
       <c r="B132" s="9">
         <v>5157879</v>
@@ -11587,28 +13710,36 @@
         <v>13</v>
       </c>
       <c r="D132" t="s" s="10">
-        <v>783</v>
+        <v>920</v>
       </c>
       <c r="E132" s="11"/>
       <c r="F132" s="11"/>
       <c r="G132" t="s" s="12">
-        <v>784</v>
+        <v>921</v>
       </c>
       <c r="H132" t="s" s="12">
         <f>HYPERLINK(G132)</f>
-        <v>785</v>
-      </c>
-      <c r="I132" s="13"/>
-      <c r="J132" s="13"/>
-      <c r="K132" s="13"/>
-      <c r="L132" s="13"/>
+        <v>922</v>
+      </c>
+      <c r="I132" t="s" s="12">
+        <v>923</v>
+      </c>
+      <c r="J132" t="s" s="12">
+        <v>924</v>
+      </c>
+      <c r="K132" t="s" s="12">
+        <v>925</v>
+      </c>
+      <c r="L132" t="s" s="12">
+        <v>926</v>
+      </c>
       <c r="M132" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="133" ht="146" customHeight="1">
       <c r="A133" t="s" s="3">
-        <v>786</v>
+        <v>927</v>
       </c>
       <c r="B133" s="9">
         <v>5148810</v>
@@ -11628,17 +13759,25 @@
         <f>HYPERLINK(G133)</f>
         <v>315</v>
       </c>
-      <c r="I133" s="13"/>
-      <c r="J133" s="13"/>
-      <c r="K133" s="13"/>
-      <c r="L133" s="13"/>
+      <c r="I133" t="s" s="12">
+        <v>928</v>
+      </c>
+      <c r="J133" t="s" s="12">
+        <v>929</v>
+      </c>
+      <c r="K133" t="s" s="12">
+        <v>930</v>
+      </c>
+      <c r="L133" t="s" s="12">
+        <v>16</v>
+      </c>
       <c r="M133" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="134" ht="159" customHeight="1">
       <c r="A134" t="s" s="3">
-        <v>787</v>
+        <v>931</v>
       </c>
       <c r="B134" s="9">
         <v>5146140</v>
@@ -11647,28 +13786,36 @@
         <v>13</v>
       </c>
       <c r="D134" t="s" s="10">
-        <v>788</v>
+        <v>932</v>
       </c>
       <c r="E134" s="11"/>
       <c r="F134" s="11"/>
       <c r="G134" t="s" s="12">
-        <v>789</v>
+        <v>933</v>
       </c>
       <c r="H134" t="s" s="12">
         <f>HYPERLINK(G134)</f>
-        <v>790</v>
-      </c>
-      <c r="I134" s="13"/>
-      <c r="J134" s="13"/>
-      <c r="K134" s="13"/>
-      <c r="L134" s="13"/>
+        <v>934</v>
+      </c>
+      <c r="I134" t="s" s="12">
+        <v>935</v>
+      </c>
+      <c r="J134" t="s" s="12">
+        <v>936</v>
+      </c>
+      <c r="K134" t="s" s="12">
+        <v>937</v>
+      </c>
+      <c r="L134" t="s" s="12">
+        <v>938</v>
+      </c>
       <c r="M134" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="135" ht="159" customHeight="1">
       <c r="A135" t="s" s="3">
-        <v>791</v>
+        <v>939</v>
       </c>
       <c r="B135" s="9">
         <v>5152101</v>
@@ -11677,28 +13824,36 @@
         <v>13</v>
       </c>
       <c r="D135" t="s" s="10">
-        <v>792</v>
+        <v>940</v>
       </c>
       <c r="E135" s="11"/>
       <c r="F135" s="11"/>
       <c r="G135" t="s" s="12">
-        <v>793</v>
+        <v>941</v>
       </c>
       <c r="H135" t="s" s="12">
         <f>HYPERLINK(G135)</f>
-        <v>794</v>
-      </c>
-      <c r="I135" s="13"/>
-      <c r="J135" s="13"/>
-      <c r="K135" s="13"/>
-      <c r="L135" s="13"/>
+        <v>942</v>
+      </c>
+      <c r="I135" t="s" s="12">
+        <v>943</v>
+      </c>
+      <c r="J135" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="K135" t="s" s="12">
+        <v>944</v>
+      </c>
+      <c r="L135" t="s" s="12">
+        <v>945</v>
+      </c>
       <c r="M135" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="136" ht="146" customHeight="1">
       <c r="A136" t="s" s="3">
-        <v>795</v>
+        <v>946</v>
       </c>
       <c r="B136" s="9">
         <v>5151991</v>
@@ -11707,28 +13862,36 @@
         <v>13</v>
       </c>
       <c r="D136" t="s" s="10">
-        <v>796</v>
+        <v>947</v>
       </c>
       <c r="E136" s="11"/>
       <c r="F136" s="11"/>
       <c r="G136" t="s" s="12">
-        <v>797</v>
+        <v>948</v>
       </c>
       <c r="H136" t="s" s="12">
         <f>HYPERLINK(G136)</f>
-        <v>798</v>
-      </c>
-      <c r="I136" s="13"/>
-      <c r="J136" s="13"/>
-      <c r="K136" s="13"/>
-      <c r="L136" s="13"/>
+        <v>949</v>
+      </c>
+      <c r="I136" t="s" s="12">
+        <v>950</v>
+      </c>
+      <c r="J136" t="s" s="12">
+        <v>951</v>
+      </c>
+      <c r="K136" t="s" s="12">
+        <v>952</v>
+      </c>
+      <c r="L136" t="s" s="12">
+        <v>953</v>
+      </c>
       <c r="M136" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="137" ht="172" customHeight="1">
       <c r="A137" t="s" s="3">
-        <v>799</v>
+        <v>954</v>
       </c>
       <c r="B137" s="9">
         <v>5147905</v>
@@ -11737,28 +13900,36 @@
         <v>13</v>
       </c>
       <c r="D137" t="s" s="10">
-        <v>800</v>
+        <v>955</v>
       </c>
       <c r="E137" s="11"/>
       <c r="F137" s="11"/>
       <c r="G137" t="s" s="12">
-        <v>801</v>
+        <v>956</v>
       </c>
       <c r="H137" t="s" s="12">
         <f>HYPERLINK(G137)</f>
-        <v>802</v>
-      </c>
-      <c r="I137" s="13"/>
-      <c r="J137" s="13"/>
-      <c r="K137" s="13"/>
-      <c r="L137" s="13"/>
+        <v>957</v>
+      </c>
+      <c r="I137" t="s" s="12">
+        <v>958</v>
+      </c>
+      <c r="J137" t="s" s="12">
+        <v>959</v>
+      </c>
+      <c r="K137" t="s" s="12">
+        <v>16</v>
+      </c>
+      <c r="L137" t="s" s="12">
+        <v>960</v>
+      </c>
       <c r="M137" t="s" s="10">
         <v>17</v>
       </c>
     </row>
     <row r="138" ht="159" customHeight="1">
       <c r="A138" t="s" s="3">
-        <v>803</v>
+        <v>961</v>
       </c>
       <c r="B138" s="9">
         <v>5156414</v>
@@ -11767,21 +13938,29 @@
         <v>13</v>
       </c>
       <c r="D138" t="s" s="10">
-        <v>804</v>
+        <v>962</v>
       </c>
       <c r="E138" s="11"/>
       <c r="F138" s="11"/>
       <c r="G138" t="s" s="12">
-        <v>805</v>
+        <v>963</v>
       </c>
       <c r="H138" t="s" s="12">
         <f>HYPERLINK(G138)</f>
-        <v>806</v>
-      </c>
-      <c r="I138" s="13"/>
-      <c r="J138" s="13"/>
-      <c r="K138" s="13"/>
-      <c r="L138" s="13"/>
+        <v>964</v>
+      </c>
+      <c r="I138" t="s" s="12">
+        <v>965</v>
+      </c>
+      <c r="J138" t="s" s="12">
+        <v>966</v>
+      </c>
+      <c r="K138" t="s" s="12">
+        <v>967</v>
+      </c>
+      <c r="L138" t="s" s="12">
+        <v>968</v>
+      </c>
       <c r="M138" t="s" s="10">
         <v>17</v>
       </c>
@@ -12146,55 +14325,218 @@
     <hyperlink ref="K88" r:id="rId356" location="" tooltip="" display="https://goo.gl/maps/NbHEfNVc4JfW8AcF7"/>
     <hyperlink ref="L88" r:id="rId357" location="" tooltip="" display="https://goo.gl/maps/FwJpum9h4AxWWFY56"/>
     <hyperlink ref="H89" r:id="rId358" location="" tooltip="" display="https://www.google.com/maps/place/HOWARD+LN+%26+WELLS+BRANCH+PKWY,+Austin,+TX"/>
-    <hyperlink ref="H90" r:id="rId359" location="" tooltip="" display="https://www.google.com/maps/place/51ST+ST+%26+35+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H91" r:id="rId360" location="" tooltip="" display="https://www.google.com/maps/place/MC+NEIL+DR+%26+PARMER+LN,+Austin,+TX"/>
-    <hyperlink ref="H92" r:id="rId361" location="" tooltip="" display="https://www.google.com/maps/place/5701+BLK+MC+NEIL+DR+,+Austin,+TX"/>
-    <hyperlink ref="H93" r:id="rId362" location="" tooltip="" display="https://www.google.com/maps/place/US+183+HWY+%26+METROPOLIS+DR,+Austin,+TX"/>
-    <hyperlink ref="H94" r:id="rId363" location="" tooltip="" display="https://www.google.com/maps/place/MENCHACA+RD+%26+SLAUGHTER+LN,+Austin,+TX"/>
-    <hyperlink ref="H95" r:id="rId364" location="" tooltip="" display="https://www.google.com/maps/place/EXPOSITION+BLVD+%26+WESTOVER+RD,+Austin,+TX"/>
-    <hyperlink ref="H96" r:id="rId365" location="" tooltip="" display="https://www.google.com/maps/place/35TH+ST+%26+KERBEY+LN,+Austin,+TX"/>
-    <hyperlink ref="H97" r:id="rId366" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+MARTIN+LUTHER+KING+JR+BLVD,+Austin,+TX"/>
-    <hyperlink ref="H98" r:id="rId367" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MEADOWS+DR,+Austin,+TX"/>
-    <hyperlink ref="H99" r:id="rId368" location="" tooltip="" display="https://www.google.com/maps/place/5501+BLK+MC+NEIL+DR+,+Austin,+TX"/>
-    <hyperlink ref="H100" r:id="rId369" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MARTIN+LUTHER+KING+JR+BLVD,+Austin,+TX"/>
-    <hyperlink ref="H101" r:id="rId370" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+KOENIG+LN+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H102" r:id="rId371" location="" tooltip="" display="https://www.google.com/maps/place/6TH+ST+%26+WEST+LYNN+ST,+Austin,+TX"/>
-    <hyperlink ref="H103" r:id="rId372" location="" tooltip="" display="https://www.google.com/maps/place/ENFIELD+RD+%26+WEST+LYNN+ST,+Austin,+TX"/>
-    <hyperlink ref="H104" r:id="rId373" location="" tooltip="" display="https://www.google.com/maps/place/ESCARPMENT+BLVD+%26+WILLIAM+CANNON+DR,+Austin,+TX"/>
-    <hyperlink ref="H105" r:id="rId374" location="" tooltip="" display="https://www.google.com/maps/place/BRODIE+LN+%26+ERNEST+ROBLES+WAY,+Austin,+TX"/>
-    <hyperlink ref="H106" r:id="rId375" location="" tooltip="" display="https://www.google.com/maps/place/51ST+ST+%26+CAMERON+RD,+Austin,+TX"/>
-    <hyperlink ref="H107" r:id="rId376" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+%26+WILLIAM+CANNON+DR,+Austin,+TX"/>
-    <hyperlink ref="H108" r:id="rId377" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MONTEREY+OAKS+BLVD,+Austin,+TX"/>
-    <hyperlink ref="H109" r:id="rId378" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H110" r:id="rId379" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H111" r:id="rId380" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H112" r:id="rId381" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+E+M+FRANKLIN+AVE,+Austin,+TX"/>
-    <hyperlink ref="H113" r:id="rId382" location="" tooltip="" display="https://www.google.com/maps/place/DESSAU+RD+%26+CRYSTAL+BEND+DR,+Austin,+TX"/>
-    <hyperlink ref="H114" r:id="rId383" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+OLD+FREDERICKSBURG+RD,+Austin,+TX"/>
-    <hyperlink ref="H115" r:id="rId384" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+%26+W+290+WB+AT+JOE+TANNER+TRN,+Austin,+TX"/>
-    <hyperlink ref="H116" r:id="rId385" location="" tooltip="" display="https://www.google.com/maps/place/7TH+ST+%26+CALLES+ST,+Austin,+TX"/>
-    <hyperlink ref="H117" r:id="rId386" location="" tooltip="" display="https://www.google.com/maps/place/2100+BLK+S+LAMAR+BLVD+,+Austin,+TX"/>
-    <hyperlink ref="H118" r:id="rId387" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+DICKSON+DR,+Austin,+TX"/>
-    <hyperlink ref="H119" r:id="rId388" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+51ST+ST,+Austin,+TX"/>
-    <hyperlink ref="H120" r:id="rId389" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+CLIFFORD+AVE,+Austin,+TX"/>
-    <hyperlink ref="H121" r:id="rId390" location="" tooltip="" display="https://www.google.com/maps/place/METRIC+BLVD+%26+KRAMER+LN,+Austin,+TX"/>
-    <hyperlink ref="H122" r:id="rId391" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+SPRINGDALE+RD,+Austin,+TX"/>
-    <hyperlink ref="H123" r:id="rId392" location="" tooltip="" display="https://www.google.com/maps/place/SPRINGDALE+RD+%26+51ST+ST,+Austin,+TX"/>
-    <hyperlink ref="H124" r:id="rId393" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+TANNEHILL+LN,+Austin,+TX"/>
-    <hyperlink ref="H125" r:id="rId394" location="" tooltip="" display="https://www.google.com/maps/place/STASSNEY+LN+%26+PALO+BLANCO+LN,+Austin,+TX"/>
-    <hyperlink ref="H126" r:id="rId395" location="" tooltip="" display="https://www.google.com/maps/place/7TH+ST+%26+PLEASANT+VALLEY+RD,+Austin,+TX"/>
-    <hyperlink ref="H127" r:id="rId396" location="" tooltip="" display="https://www.google.com/maps/place/CESAR+CHAVEZ+ST+%26+COMAL+ST,+Austin,+TX"/>
-    <hyperlink ref="H128" r:id="rId397" location="" tooltip="" display="https://www.google.com/maps/place/PARMER+LN+%26+SPECTRUM+DR,+Austin,+TX"/>
-    <hyperlink ref="H129" r:id="rId398" location="" tooltip="" display="https://www.google.com/maps/place/35TH+ST+%26+JACKSON+AVE,+Austin,+TX"/>
-    <hyperlink ref="H130" r:id="rId399" location="" tooltip="" display="https://www.google.com/maps/place/FM+620+RD+%26+PARMER+LN,+Austin,+TX"/>
-    <hyperlink ref="H131" r:id="rId400" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+BLUEBONNET+LN,+Austin,+TX"/>
-    <hyperlink ref="H132" r:id="rId401" location="" tooltip="" display="https://www.google.com/maps/place/STASSNEY+LN+%26+NUCKOLS+CROSSING+RD,+Austin,+TX"/>
-    <hyperlink ref="H133" r:id="rId402" location="" tooltip="" display="https://www.google.com/maps/place/BRODIE+LN+%26+290+HWY+SVRD,+Austin,+TX"/>
-    <hyperlink ref="H134" r:id="rId403" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+FOSTER+RANCH+RD,+Austin,+TX"/>
-    <hyperlink ref="H135" r:id="rId404" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MENCHACA+RD+,+Austin,+TX"/>
-    <hyperlink ref="H136" r:id="rId405" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+BARTON+SKWY+,+Austin,+TX"/>
-    <hyperlink ref="H137" r:id="rId406" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+REPUBLIC+OF+TEXAS+BLVD,+Austin,+TX"/>
-    <hyperlink ref="H138" r:id="rId407" location="" tooltip="" display="https://www.google.com/maps/place/SHOAL+CREEK+BLVD+%26+HANCOCK+DR,+Austin,+TX"/>
+    <hyperlink ref="J89" r:id="rId359" location="" tooltip="" display="https://goo.gl/maps/CS19pRmU3gJvKiSv9"/>
+    <hyperlink ref="K89" r:id="rId360" location="" tooltip="" display="https://goo.gl/maps/7Y12NQ8tbZDtrHiz8"/>
+    <hyperlink ref="L89" r:id="rId361" location="" tooltip="" display="https://goo.gl/maps/xVxF4b3tUmHAKMCE9"/>
+    <hyperlink ref="H90" r:id="rId362" location="" tooltip="" display="https://www.google.com/maps/place/51ST+ST+%26+35+SVRD,+Austin,+TX"/>
+    <hyperlink ref="H91" r:id="rId363" location="" tooltip="" display="https://www.google.com/maps/place/MC+NEIL+DR+%26+PARMER+LN,+Austin,+TX"/>
+    <hyperlink ref="I91" r:id="rId364" location="" tooltip="" display="https://goo.gl/maps/W7UxkkJhqgTgNyT17"/>
+    <hyperlink ref="J91" r:id="rId365" location="" tooltip="" display="https://goo.gl/maps/5mYp1amfqHR7CKJ17"/>
+    <hyperlink ref="K91" r:id="rId366" location="" tooltip="" display="https://goo.gl/maps/F8bpjpz4z4XAN4kT9"/>
+    <hyperlink ref="L91" r:id="rId367" location="" tooltip="" display="https://goo.gl/maps/KHrbz8LRWemLN83QA"/>
+    <hyperlink ref="H92" r:id="rId368" location="" tooltip="" display="https://www.google.com/maps/place/5701+BLK+MC+NEIL+DR+,+Austin,+TX"/>
+    <hyperlink ref="I92" r:id="rId369" location="" tooltip="" display="https://goo.gl/maps/hfT1DmqpAnDbTo9Z7"/>
+    <hyperlink ref="J92" r:id="rId370" location="" tooltip="" display="https://goo.gl/maps/ZMWFV1TCHDSywfrq5"/>
+    <hyperlink ref="K92" r:id="rId371" location="" tooltip="" display="https://goo.gl/maps/ESC88einSeu47hNv8"/>
+    <hyperlink ref="L92" r:id="rId372" location="" tooltip="" display="https://goo.gl/maps/Dsc8t3zEiNfS5sHg8"/>
+    <hyperlink ref="H93" r:id="rId373" location="" tooltip="" display="https://www.google.com/maps/place/US+183+HWY+%26+METROPOLIS+DR,+Austin,+TX"/>
+    <hyperlink ref="I93" r:id="rId374" location="" tooltip="" display="https://goo.gl/maps/EedipFgGpoZ7R4UX9"/>
+    <hyperlink ref="J93" r:id="rId375" location="" tooltip="" display="https://goo.gl/maps/FgihyCUixopkwFBK8"/>
+    <hyperlink ref="K93" r:id="rId376" location="" tooltip="" display="https://goo.gl/maps/Uw5AsZ1zKvdY9i5t5"/>
+    <hyperlink ref="H94" r:id="rId377" location="" tooltip="" display="https://www.google.com/maps/place/MENCHACA+RD+%26+SLAUGHTER+LN,+Austin,+TX"/>
+    <hyperlink ref="I94" r:id="rId378" location="" tooltip="" display="https://goo.gl/maps/aghpT5hHmPWqHyhB7"/>
+    <hyperlink ref="J94" r:id="rId379" location="" tooltip="" display="https://goo.gl/maps/pGMuWGUR55dmvQ1s5"/>
+    <hyperlink ref="K94" r:id="rId380" location="" tooltip="" display="https://goo.gl/maps/sUe4WPttT8djc8y88"/>
+    <hyperlink ref="L94" r:id="rId381" location="" tooltip="" display="https://goo.gl/maps/AaZBhvMWLyrDaxsL8"/>
+    <hyperlink ref="H95" r:id="rId382" location="" tooltip="" display="https://www.google.com/maps/place/EXPOSITION+BLVD+%26+WESTOVER+RD,+Austin,+TX"/>
+    <hyperlink ref="I95" r:id="rId383" location="" tooltip="" display="https://goo.gl/maps/ZMXdf3m5B9sNkGWFA"/>
+    <hyperlink ref="J95" r:id="rId384" location="" tooltip="" display="https://goo.gl/maps/PZV1WZuVL9BzTK4Z8"/>
+    <hyperlink ref="K95" r:id="rId385" location="" tooltip="" display="https://goo.gl/maps/4JoSKjZxQsFXn49v6"/>
+    <hyperlink ref="L95" r:id="rId386" location="" tooltip="" display="https://goo.gl/maps/uh22JNTVD1wpJ6qi8"/>
+    <hyperlink ref="H96" r:id="rId387" location="" tooltip="" display="https://www.google.com/maps/place/35TH+ST+%26+KERBEY+LN,+Austin,+TX"/>
+    <hyperlink ref="I96" r:id="rId388" location="" tooltip="" display="https://goo.gl/maps/jHXmuhJLxkDfMjxi7"/>
+    <hyperlink ref="K96" r:id="rId389" location="" tooltip="" display="https://goo.gl/maps/gXqKjgArVTWE18X67"/>
+    <hyperlink ref="L96" r:id="rId390" location="" tooltip="" display="https://goo.gl/maps/J2DKCiHvVs1PtBDS8"/>
+    <hyperlink ref="H97" r:id="rId391" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+MARTIN+LUTHER+KING+JR+BLVD,+Austin,+TX"/>
+    <hyperlink ref="I97" r:id="rId392" location="" tooltip="" display="https://goo.gl/maps/YnMYTqrysmZeNCmw8"/>
+    <hyperlink ref="J97" r:id="rId393" location="" tooltip="" display="https://goo.gl/maps/T4bEb9dxN8tj4fUG7"/>
+    <hyperlink ref="K97" r:id="rId394" location="" tooltip="" display="https://goo.gl/maps/PJ2zUC7dxZHgRroS7"/>
+    <hyperlink ref="L97" r:id="rId395" location="" tooltip="" display="https://goo.gl/maps/DzgXDnjtxeZihT2s5"/>
+    <hyperlink ref="H98" r:id="rId396" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MEADOWS+DR,+Austin,+TX"/>
+    <hyperlink ref="I98" r:id="rId397" location="" tooltip="" display="https://goo.gl/maps/xJEZScTM3jd31vjv7"/>
+    <hyperlink ref="J98" r:id="rId398" location="" tooltip="" display="https://goo.gl/maps/7igom4JU6M4SNSuBA"/>
+    <hyperlink ref="K98" r:id="rId399" location="" tooltip="" display="https://goo.gl/maps/ESTyDw9Lut2NS5Hs9"/>
+    <hyperlink ref="L98" r:id="rId400" location="" tooltip="" display="https://goo.gl/maps/KAPdszwxyKekKeaz7"/>
+    <hyperlink ref="H99" r:id="rId401" location="" tooltip="" display="https://www.google.com/maps/place/5501+BLK+MC+NEIL+DR+,+Austin,+TX"/>
+    <hyperlink ref="I99" r:id="rId402" location="" tooltip="" display="https://goo.gl/maps/Y5VnGD6uDHWBNnX18"/>
+    <hyperlink ref="J99" r:id="rId403" location="" tooltip="" display="https://goo.gl/maps/WUcmGJsgfRU2mSDLA"/>
+    <hyperlink ref="K99" r:id="rId404" location="" tooltip="" display="https://goo.gl/maps/ESTyDw9Lut2NS5Hs9"/>
+    <hyperlink ref="L99" r:id="rId405" location="" tooltip="" display="https://goo.gl/maps/v3aTBeaPY8xay8H78"/>
+    <hyperlink ref="H100" r:id="rId406" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MARTIN+LUTHER+KING+JR+BLVD,+Austin,+TX"/>
+    <hyperlink ref="I100" r:id="rId407" location="" tooltip="" display="https://goo.gl/maps/bD5sgWGFfpPR3g6G8"/>
+    <hyperlink ref="J100" r:id="rId408" location="" tooltip="" display="https://goo.gl/maps/q4C3jXjr6U9KavAu6"/>
+    <hyperlink ref="L100" r:id="rId409" location="" tooltip="" display="https://goo.gl/maps/q51dSkwJwMzQBsod6"/>
+    <hyperlink ref="H101" r:id="rId410" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+KOENIG+LN+SVRD,+Austin,+TX"/>
+    <hyperlink ref="I101" r:id="rId411" location="" tooltip="" display="https://goo.gl/maps/auCxBooZmFBN6moA9"/>
+    <hyperlink ref="J101" r:id="rId412" location="" tooltip="" display="https://goo.gl/maps/AdVE4j5KNAqK3PZy5"/>
+    <hyperlink ref="L101" r:id="rId413" location="" tooltip="" display="https://goo.gl/maps/tmTrmsuNtbW9fj3i7"/>
+    <hyperlink ref="H102" r:id="rId414" location="" tooltip="" display="https://www.google.com/maps/place/6TH+ST+%26+WEST+LYNN+ST,+Austin,+TX"/>
+    <hyperlink ref="I102" r:id="rId415" location="" tooltip="" display="https://goo.gl/maps/S47N95nvEgJiveT1A"/>
+    <hyperlink ref="J102" r:id="rId416" location="" tooltip="" display="https://goo.gl/maps/xDbHjRoqKYdCa55g9"/>
+    <hyperlink ref="L102" r:id="rId417" location="" tooltip="" display="https://goo.gl/maps/aoKoSpsUKKyAh4ez6"/>
+    <hyperlink ref="H103" r:id="rId418" location="" tooltip="" display="https://www.google.com/maps/place/ENFIELD+RD+%26+WEST+LYNN+ST,+Austin,+TX"/>
+    <hyperlink ref="I103" r:id="rId419" location="" tooltip="" display="https://goo.gl/maps/z4dwugxPNoPRyLzV7"/>
+    <hyperlink ref="J103" r:id="rId420" location="" tooltip="" display="https://goo.gl/maps/QbB6B5XNEzRPLcRW6"/>
+    <hyperlink ref="K103" r:id="rId421" location="" tooltip="" display="https://goo.gl/maps/fcBcNbaxxYwhz5NA7"/>
+    <hyperlink ref="L103" r:id="rId422" location="" tooltip="" display="https://goo.gl/maps/DFU3CVug9eL7srUr7"/>
+    <hyperlink ref="H104" r:id="rId423" location="" tooltip="" display="https://www.google.com/maps/place/ESCARPMENT+BLVD+%26+WILLIAM+CANNON+DR,+Austin,+TX"/>
+    <hyperlink ref="I104" r:id="rId424" location="" tooltip="" display="https://goo.gl/maps/19AXTpeHCQAS9d6m9"/>
+    <hyperlink ref="J104" r:id="rId425" location="" tooltip="" display="https://goo.gl/maps/uWpGrAuSPSMG71mJA"/>
+    <hyperlink ref="K104" r:id="rId426" location="" tooltip="" display="https://goo.gl/maps/kRFE8fvmB7HwQe2E8"/>
+    <hyperlink ref="L104" r:id="rId427" location="" tooltip="" display="https://goo.gl/maps/RjxBLNgiN55phzrU7"/>
+    <hyperlink ref="H105" r:id="rId428" location="" tooltip="" display="https://www.google.com/maps/place/BRODIE+LN+%26+ERNEST+ROBLES+WAY,+Austin,+TX"/>
+    <hyperlink ref="I105" r:id="rId429" location="" tooltip="" display="https://goo.gl/maps/vzwq8aW5mKKc5DgJ8"/>
+    <hyperlink ref="J105" r:id="rId430" location="" tooltip="" display="https://goo.gl/maps/vNNzLE8MaTEkmsBV6"/>
+    <hyperlink ref="K105" r:id="rId431" location="" tooltip="" display="https://goo.gl/maps/KZxRXdQTzbqtBJMz7"/>
+    <hyperlink ref="L105" r:id="rId432" location="" tooltip="" display="https://goo.gl/maps/vU2yu3nvERJDkhdc9"/>
+    <hyperlink ref="H106" r:id="rId433" location="" tooltip="" display="https://www.google.com/maps/place/51ST+ST+%26+CAMERON+RD,+Austin,+TX"/>
+    <hyperlink ref="J106" r:id="rId434" location="" tooltip="" display="https://goo.gl/maps/WBgpBev5rPLWwjP38"/>
+    <hyperlink ref="K106" r:id="rId435" location="" tooltip="" display="https://goo.gl/maps/6CsB2w6jrVswkrrd8"/>
+    <hyperlink ref="L106" r:id="rId436" location="" tooltip="" display="https://goo.gl/maps/fTH5RoqhmhGeFw6b7"/>
+    <hyperlink ref="H107" r:id="rId437" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+%26+WILLIAM+CANNON+DR,+Austin,+TX"/>
+    <hyperlink ref="I107" r:id="rId438" location="" tooltip="" display="https://goo.gl/maps/eSGV5XZLEGWhQexZ6"/>
+    <hyperlink ref="J107" r:id="rId439" location="" tooltip="" display="https://goo.gl/maps/XeGwregfm1xHc9Hm8"/>
+    <hyperlink ref="K107" r:id="rId440" location="" tooltip="" display="https://goo.gl/maps/MaJWfHaZDKjN252U8"/>
+    <hyperlink ref="L107" r:id="rId441" location="" tooltip="" display="https://goo.gl/maps/T9vHpRYJg6moH5hH7"/>
+    <hyperlink ref="H108" r:id="rId442" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MONTEREY+OAKS+BLVD,+Austin,+TX"/>
+    <hyperlink ref="I108" r:id="rId443" location="" tooltip="" display="https://goo.gl/maps/DMPSctVAjFQCY9Rh8"/>
+    <hyperlink ref="J108" r:id="rId444" location="" tooltip="" display="https://goo.gl/maps/aoxZQED2KcPQ6zfS9"/>
+    <hyperlink ref="K108" r:id="rId445" location="" tooltip="" display="https://goo.gl/maps/QqLPFb67qcmfvsbD9"/>
+    <hyperlink ref="H109" r:id="rId446" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
+    <hyperlink ref="I109" r:id="rId447" location="" tooltip="" display="https://goo.gl/maps/DoKyNBiWYqZCiLKW6"/>
+    <hyperlink ref="K109" r:id="rId448" location="" tooltip="" display="https://goo.gl/maps/C1Yfhnw6pFdKKT6s5"/>
+    <hyperlink ref="H110" r:id="rId449" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
+    <hyperlink ref="J110" r:id="rId450" location="" tooltip="" display="https://goo.gl/maps/J2PArsKwDnzNsfnq7"/>
+    <hyperlink ref="K110" r:id="rId451" location="" tooltip="" display="https://goo.gl/maps/8x5AigDmeCx2Qxsm7"/>
+    <hyperlink ref="H111" r:id="rId452" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+MOPAC+EXPY+SVRD,+Austin,+TX"/>
+    <hyperlink ref="I111" r:id="rId453" location="" tooltip="" display="https://goo.gl/maps/P8CR1UKYEbrXCka4A"/>
+    <hyperlink ref="J111" r:id="rId454" location="" tooltip="" display="https://goo.gl/maps/AMfTdUj5P5ipvTyg9"/>
+    <hyperlink ref="L111" r:id="rId455" location="" tooltip="" display="https://goo.gl/maps/QRqgFYhSBYVNHBS87"/>
+    <hyperlink ref="H112" r:id="rId456" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+E+M+FRANKLIN+AVE,+Austin,+TX"/>
+    <hyperlink ref="I112" r:id="rId457" location="" tooltip="" display="https://goo.gl/maps/56dbeokQKXSUpF7BA"/>
+    <hyperlink ref="J112" r:id="rId458" location="" tooltip="" display="https://goo.gl/maps/znKJA51SgWj84QrF8"/>
+    <hyperlink ref="K112" r:id="rId459" location="" tooltip="" display="https://goo.gl/maps/iMcm945afhbM9EiB9"/>
+    <hyperlink ref="L112" r:id="rId460" location="" tooltip="" display="https://goo.gl/maps/iz29tDGmqTENPUNv6"/>
+    <hyperlink ref="H113" r:id="rId461" location="" tooltip="" display="https://www.google.com/maps/place/DESSAU+RD+%26+CRYSTAL+BEND+DR,+Austin,+TX"/>
+    <hyperlink ref="I113" r:id="rId462" location="" tooltip="" display="https://goo.gl/maps/RT7m4Y3Fu1yGRGP58"/>
+    <hyperlink ref="J113" r:id="rId463" location="" tooltip="" display="https://goo.gl/maps/shuwK4WWkyqenC9R6"/>
+    <hyperlink ref="K113" r:id="rId464" location="" tooltip="" display="https://goo.gl/maps/nDLurtQfMcrpZxh56"/>
+    <hyperlink ref="L113" r:id="rId465" location="" tooltip="" display="https://goo.gl/maps/xSUAH6aRJpu97wEL9"/>
+    <hyperlink ref="H114" r:id="rId466" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+SVRD+%26+OLD+FREDERICKSBURG+RD,+Austin,+TX"/>
+    <hyperlink ref="I114" r:id="rId467" location="" tooltip="" display="https://goo.gl/maps/5iD4jhvXe1LEejHf9"/>
+    <hyperlink ref="J114" r:id="rId468" location="" tooltip="" display="https://goo.gl/maps/KJjsfEVd2n7TSmrE7"/>
+    <hyperlink ref="K114" r:id="rId469" location="" tooltip="" display="https://goo.gl/maps/5Jc4UZHzqZzbfDMo6"/>
+    <hyperlink ref="H115" r:id="rId470" location="" tooltip="" display="https://www.google.com/maps/place/US+290+HWY+%26+W+290+WB+AT+JOE+TANNER+TRN,+Austin,+TX"/>
+    <hyperlink ref="J115" r:id="rId471" location="" tooltip="" display="https://goo.gl/maps/sBonvkz7BpL5qfv28"/>
+    <hyperlink ref="K115" r:id="rId472" location="" tooltip="" display="https://goo.gl/maps/wzz6E4jL3DuBuYaUA"/>
+    <hyperlink ref="H116" r:id="rId473" location="" tooltip="" display="https://www.google.com/maps/place/7TH+ST+%26+CALLES+ST,+Austin,+TX"/>
+    <hyperlink ref="K116" r:id="rId474" location="" tooltip="" display="https://goo.gl/maps/NRMC6JmvSFFHcMNm9"/>
+    <hyperlink ref="L116" r:id="rId475" location="" tooltip="" display="https://goo.gl/maps/6dvSYQ5LUK82UtyQ8"/>
+    <hyperlink ref="H117" r:id="rId476" location="" tooltip="" display="https://www.google.com/maps/place/2100+BLK+S+LAMAR+BLVD+,+Austin,+TX"/>
+    <hyperlink ref="H118" r:id="rId477" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+DICKSON+DR,+Austin,+TX"/>
+    <hyperlink ref="I118" r:id="rId478" location="" tooltip="" display="https://goo.gl/maps/R1h5KXYWm7cNpuLT7"/>
+    <hyperlink ref="J118" r:id="rId479" location="" tooltip="" display="https://goo.gl/maps/ce1ch7dgTAoa8eS99"/>
+    <hyperlink ref="H119" r:id="rId480" location="" tooltip="" display="https://www.google.com/maps/place/AIRPORT+BLVD+%26+51ST+ST,+Austin,+TX"/>
+    <hyperlink ref="I119" r:id="rId481" location="" tooltip="" display="https://goo.gl/maps/a8hDhn451US6ZJKg7"/>
+    <hyperlink ref="J119" r:id="rId482" location="" tooltip="" display="https://goo.gl/maps/BGtnkD9wFUFjmocR8"/>
+    <hyperlink ref="K119" r:id="rId483" location="" tooltip="" display="https://goo.gl/maps/H5EvCrzdfHc1s4RW6"/>
+    <hyperlink ref="L119" r:id="rId484" location="" tooltip="" display="https://goo.gl/maps/mFecJFq9tzP6VNcR8"/>
+    <hyperlink ref="H120" r:id="rId485" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+CLIFFORD+AVE,+Austin,+TX"/>
+    <hyperlink ref="H121" r:id="rId486" location="" tooltip="" display="https://www.google.com/maps/place/METRIC+BLVD+%26+KRAMER+LN,+Austin,+TX"/>
+    <hyperlink ref="I121" r:id="rId487" location="" tooltip="" display="https://goo.gl/maps/8bw6R341ynynUv4w5"/>
+    <hyperlink ref="J121" r:id="rId488" location="" tooltip="" display="https://goo.gl/maps/AGVzgZPLMg5Khrg8A"/>
+    <hyperlink ref="K121" r:id="rId489" location="" tooltip="" display="https://goo.gl/maps/v677GYGfavVSaqs29"/>
+    <hyperlink ref="L121" r:id="rId490" location="" tooltip="" display="https://goo.gl/maps/WrJri2Xpm25fdCBs7"/>
+    <hyperlink ref="H122" r:id="rId491" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+SPRINGDALE+RD,+Austin,+TX"/>
+    <hyperlink ref="I122" r:id="rId492" location="" tooltip="" display="https://goo.gl/maps/7Ga3AYBNncQXA35TA"/>
+    <hyperlink ref="J122" r:id="rId493" location="" tooltip="" display="https://goo.gl/maps/HMWefQZN3GThMjK16"/>
+    <hyperlink ref="K122" r:id="rId494" location="" tooltip="" display="https://goo.gl/maps/mnbzF1kKHoATFqmh8"/>
+    <hyperlink ref="L122" r:id="rId495" location="" tooltip="" display="https://goo.gl/maps/PELtMYbJ4VcAxysC9"/>
+    <hyperlink ref="H123" r:id="rId496" location="" tooltip="" display="https://www.google.com/maps/place/SPRINGDALE+RD+%26+51ST+ST,+Austin,+TX"/>
+    <hyperlink ref="I123" r:id="rId497" location="" tooltip="" display="https://goo.gl/maps/firaP6nr2Z9RDbCX8"/>
+    <hyperlink ref="J123" r:id="rId498" location="" tooltip="" display="https://goo.gl/maps/endg7BJUZE383Ldo7"/>
+    <hyperlink ref="K123" r:id="rId499" location="" tooltip="" display="https://goo.gl/maps/XJaJkwwNkuNyxKdw9"/>
+    <hyperlink ref="L123" r:id="rId500" location="" tooltip="" display="https://goo.gl/maps/mzMwLmoaCpE7ZaWv9"/>
+    <hyperlink ref="H124" r:id="rId501" location="" tooltip="" display="https://www.google.com/maps/place/MARTIN+LUTHER+KING+JR+BLVD+%26+TANNEHILL+LN,+Austin,+TX"/>
+    <hyperlink ref="I124" r:id="rId502" location="" tooltip="" display="https://goo.gl/maps/wMp9GHyejd3qKxJn7"/>
+    <hyperlink ref="J124" r:id="rId503" location="" tooltip="" display="https://goo.gl/maps/d2hk7tJGSZ52Yoan9"/>
+    <hyperlink ref="K124" r:id="rId504" location="" tooltip="" display="https://goo.gl/maps/kF3N6cStuvkajBpv5"/>
+    <hyperlink ref="L124" r:id="rId505" location="" tooltip="" display="https://goo.gl/maps/JwCfSa3cukU3Hcjq6"/>
+    <hyperlink ref="H125" r:id="rId506" location="" tooltip="" display="https://www.google.com/maps/place/STASSNEY+LN+%26+PALO+BLANCO+LN,+Austin,+TX"/>
+    <hyperlink ref="I125" r:id="rId507" location="" tooltip="" display="https://goo.gl/maps/ig3TBVi1toXCtFjd9"/>
+    <hyperlink ref="J125" r:id="rId508" location="" tooltip="" display="https://goo.gl/maps/bnH4qomUk4TBmxkHA"/>
+    <hyperlink ref="K125" r:id="rId509" location="" tooltip="" display="https://goo.gl/maps/5jj5uWuAhRFjHcxW8"/>
+    <hyperlink ref="L125" r:id="rId510" location="" tooltip="" display="https://goo.gl/maps/zNMSYRYv2SNsRsAT7"/>
+    <hyperlink ref="H126" r:id="rId511" location="" tooltip="" display="https://www.google.com/maps/place/7TH+ST+%26+PLEASANT+VALLEY+RD,+Austin,+TX"/>
+    <hyperlink ref="I126" r:id="rId512" location="" tooltip="" display="https://goo.gl/maps/6BitBhpGfwB3pMoQ8"/>
+    <hyperlink ref="J126" r:id="rId513" location="" tooltip="" display="https://goo.gl/maps/5LqR3NoVdF6938cQA"/>
+    <hyperlink ref="K126" r:id="rId514" location="" tooltip="" display="https://goo.gl/maps/EoMEnssG9KRaPhtV7"/>
+    <hyperlink ref="L126" r:id="rId515" location="" tooltip="" display="https://goo.gl/maps/ayGHikfeLMQEi7bS6"/>
+    <hyperlink ref="H127" r:id="rId516" location="" tooltip="" display="https://www.google.com/maps/place/CESAR+CHAVEZ+ST+%26+COMAL+ST,+Austin,+TX"/>
+    <hyperlink ref="I127" r:id="rId517" location="" tooltip="" display="https://goo.gl/maps/yvYBmWAqAas9GQ7e8"/>
+    <hyperlink ref="J127" r:id="rId518" location="" tooltip="" display="https://goo.gl/maps/f3uUrzWRxG6s17rC8"/>
+    <hyperlink ref="K127" r:id="rId519" location="" tooltip="" display="https://goo.gl/maps/gwYNgqoNB1kjs6vs7"/>
+    <hyperlink ref="L127" r:id="rId520" location="" tooltip="" display="https://goo.gl/maps/L94X64ydjkVMknYD6"/>
+    <hyperlink ref="H128" r:id="rId521" location="" tooltip="" display="https://www.google.com/maps/place/PARMER+LN+%26+SPECTRUM+DR,+Austin,+TX"/>
+    <hyperlink ref="I128" r:id="rId522" location="" tooltip="" display="https://goo.gl/maps/ocVnT59W8mgUWpXb9"/>
+    <hyperlink ref="J128" r:id="rId523" location="" tooltip="" display="https://goo.gl/maps/HGKsYrbgHF2ayee48"/>
+    <hyperlink ref="K128" r:id="rId524" location="" tooltip="" display="https://goo.gl/maps/9SRR2tn1UGLu3RWj9"/>
+    <hyperlink ref="L128" r:id="rId525" location="" tooltip="" display="https://goo.gl/maps/roJ876eHfV4zm8wNA"/>
+    <hyperlink ref="H129" r:id="rId526" location="" tooltip="" display="https://www.google.com/maps/place/35TH+ST+%26+JACKSON+AVE,+Austin,+TX"/>
+    <hyperlink ref="I129" r:id="rId527" location="" tooltip="" display="https://goo.gl/maps/v76u7Y1J1Ah3ENuV7"/>
+    <hyperlink ref="J129" r:id="rId528" location="" tooltip="" display="https://goo.gl/maps/Yb5BMDdgtdYxGTxB7"/>
+    <hyperlink ref="K129" r:id="rId529" location="" tooltip="" display="https://goo.gl/maps/8BbJY6LXpKbQzMVdA"/>
+    <hyperlink ref="L129" r:id="rId530" location="" tooltip="" display="https://goo.gl/maps/oxKyF8fahfxedqgF8"/>
+    <hyperlink ref="H130" r:id="rId531" location="" tooltip="" display="https://www.google.com/maps/place/FM+620+RD+%26+PARMER+LN,+Austin,+TX"/>
+    <hyperlink ref="I130" r:id="rId532" location="" tooltip="" display="https://goo.gl/maps/c9MQ22rnDgXkK6JA8"/>
+    <hyperlink ref="J130" r:id="rId533" location="" tooltip="" display="https://goo.gl/maps/fFs7EzcCfVDeNo9e6"/>
+    <hyperlink ref="K130" r:id="rId534" location="" tooltip="" display="https://goo.gl/maps/by4T44ZZkX8t2GQT7"/>
+    <hyperlink ref="H131" r:id="rId535" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+BLUEBONNET+LN,+Austin,+TX"/>
+    <hyperlink ref="I131" r:id="rId536" location="" tooltip="" display="https://goo.gl/maps/iKaCZdAFmcT32Q8s7"/>
+    <hyperlink ref="K131" r:id="rId537" location="" tooltip="" display="https://goo.gl/maps/qVU8LL3mKveW3ZPW6"/>
+    <hyperlink ref="L131" r:id="rId538" location="" tooltip="" display="https://goo.gl/maps/FpHjYFVJQM6YUevLA"/>
+    <hyperlink ref="H132" r:id="rId539" location="" tooltip="" display="https://www.google.com/maps/place/STASSNEY+LN+%26+NUCKOLS+CROSSING+RD,+Austin,+TX"/>
+    <hyperlink ref="I132" r:id="rId540" location="" tooltip="" display="https://goo.gl/maps/EvYtRfBRU7rbWhrZA"/>
+    <hyperlink ref="J132" r:id="rId541" location="" tooltip="" display="https://goo.gl/maps/PBEXL3ptu82zdTtt9"/>
+    <hyperlink ref="K132" r:id="rId542" location="" tooltip="" display="https://goo.gl/maps/hh8PZFMiajiEBDNi6"/>
+    <hyperlink ref="L132" r:id="rId543" location="" tooltip="" display="https://goo.gl/maps/ukxxLScnKgHYykYU9"/>
+    <hyperlink ref="H133" r:id="rId544" location="" tooltip="" display="https://www.google.com/maps/place/BRODIE+LN+%26+290+HWY+SVRD,+Austin,+TX"/>
+    <hyperlink ref="I133" r:id="rId545" location="" tooltip="" display="https://goo.gl/maps/TgZdLynmEegdMKhD9"/>
+    <hyperlink ref="J133" r:id="rId546" location="" tooltip="" display="https://goo.gl/maps/6WPHDfofA4iU3UBh9"/>
+    <hyperlink ref="K133" r:id="rId547" location="" tooltip="" display="https://goo.gl/maps/3dRkw43X1wYuSUKG9"/>
+    <hyperlink ref="H134" r:id="rId548" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+FOSTER+RANCH+RD,+Austin,+TX"/>
+    <hyperlink ref="I134" r:id="rId549" location="" tooltip="" display="https://goo.gl/maps/4b5C1GKrMSDJ5dDi8"/>
+    <hyperlink ref="J134" r:id="rId550" location="" tooltip="" display="https://goo.gl/maps/UMHeTH8qM9nD4pne8"/>
+    <hyperlink ref="K134" r:id="rId551" location="" tooltip="" display="https://goo.gl/maps/WHTJAgza4Akop8GS9"/>
+    <hyperlink ref="L134" r:id="rId552" location="" tooltip="" display="https://goo.gl/maps/HUzUNs6LoY1bddet5"/>
+    <hyperlink ref="H135" r:id="rId553" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+MENCHACA+RD+,+Austin,+TX"/>
+    <hyperlink ref="I135" r:id="rId554" location="" tooltip="" display="https://goo.gl/maps/sibKoAey5HWpCXuM9"/>
+    <hyperlink ref="K135" r:id="rId555" location="" tooltip="" display="https://goo.gl/maps/an1ZsoTPPHTu9HFKA"/>
+    <hyperlink ref="L135" r:id="rId556" location="" tooltip="" display="https://goo.gl/maps/7qhwJ9DpxQodnxaRA"/>
+    <hyperlink ref="H136" r:id="rId557" location="" tooltip="" display="https://www.google.com/maps/place/LAMAR+BLVD+%26+BARTON+SKWY+,+Austin,+TX"/>
+    <hyperlink ref="I136" r:id="rId558" location="" tooltip="" display="https://goo.gl/maps/n19VqbzBeF9KJgfW6"/>
+    <hyperlink ref="J136" r:id="rId559" location="" tooltip="" display="https://goo.gl/maps/yAxUZUpCeGFT1Ehj6"/>
+    <hyperlink ref="K136" r:id="rId560" location="" tooltip="" display="https://goo.gl/maps/CdGzmfvr8fNLzZnj6"/>
+    <hyperlink ref="L136" r:id="rId561" location="" tooltip="" display="https://goo.gl/maps/zbTtfcd6Hqckytx3A"/>
+    <hyperlink ref="H137" r:id="rId562" location="" tooltip="" display="https://www.google.com/maps/place/SOUTHWEST+PKWY+%26+REPUBLIC+OF+TEXAS+BLVD,+Austin,+TX"/>
+    <hyperlink ref="I137" r:id="rId563" location="" tooltip="" display="https://goo.gl/maps/683aFsUn4uDTtxqW8"/>
+    <hyperlink ref="J137" r:id="rId564" location="" tooltip="" display="https://goo.gl/maps/7USBcXtzPJrBd7R8A"/>
+    <hyperlink ref="L137" r:id="rId565" location="" tooltip="" display="https://goo.gl/maps/5erjFkQffpEj7b718"/>
+    <hyperlink ref="H138" r:id="rId566" location="" tooltip="" display="https://www.google.com/maps/place/SHOAL+CREEK+BLVD+%26+HANCOCK+DR,+Austin,+TX"/>
+    <hyperlink ref="I138" r:id="rId567" location="" tooltip="" display="https://goo.gl/maps/8t12iujeT587qSm56"/>
+    <hyperlink ref="J138" r:id="rId568" location="" tooltip="" display="https://goo.gl/maps/oAoDCHz7SMhhcSmo8"/>
+    <hyperlink ref="K138" r:id="rId569" location="" tooltip="" display="https://goo.gl/maps/GU4Q5b1gvgVXQ7gU6"/>
+    <hyperlink ref="L138" r:id="rId570" location="" tooltip="" display="https://goo.gl/maps/2kurqLrzeM57gwKz8"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>